<commit_message>
add more regression models and chart
</commit_message>
<xml_diff>
--- a/OUTPUT/DATA/Charting.xlsx
+++ b/OUTPUT/DATA/Charting.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="M:\Work\Childcare and parental employment\childcare\OUTPUT\DATA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F87821C-02EB-493A-9534-123351B57E57}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E065364-C4C8-4BDC-AEF7-9E917FED4458}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-5780" yWindow="-21710" windowWidth="38620" windowHeight="21220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-3735" yWindow="8002" windowWidth="20715" windowHeight="13276" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="34">
   <si>
     <t>Barchart showing employment rates, parents vs. non-parents, by overall, sex and region</t>
   </si>
@@ -619,9 +619,6 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="164" fontId="2" fillId="0" borderId="16" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="3" fontId="2" fillId="0" borderId="18" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="2" fillId="0" borderId="17" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
@@ -653,11 +650,14 @@
     <xf numFmtId="3" fontId="2" fillId="0" borderId="18" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="165" fontId="2" fillId="0" borderId="22" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="3" fontId="2" fillId="0" borderId="22" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1539,7 +1539,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$C$38</c:f>
+              <c:f>Sheet1!$C$53</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1564,7 +1564,7 @@
             <c:noEndCap val="0"/>
             <c:plus>
               <c:numRef>
-                <c:f>Sheet1!$D$40:$D$44</c:f>
+                <c:f>Sheet1!$D$55:$D$59</c:f>
                 <c:numCache>
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="5"/>
@@ -1588,7 +1588,7 @@
             </c:plus>
             <c:minus>
               <c:numRef>
-                <c:f>Sheet1!$D$40:$D$44</c:f>
+                <c:f>Sheet1!$D$55:$D$59</c:f>
                 <c:numCache>
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="5"/>
@@ -1626,7 +1626,7 @@
           </c:errBars>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$B$40:$B$44</c:f>
+              <c:f>Sheet1!$B$55:$B$59</c:f>
               <c:strCache>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
@@ -1649,7 +1649,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$C$40:$C$44</c:f>
+              <c:f>Sheet1!$C$55:$C$59</c:f>
               <c:numCache>
                 <c:formatCode>0.0%</c:formatCode>
                 <c:ptCount val="5"/>
@@ -1682,7 +1682,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$F$38</c:f>
+              <c:f>Sheet1!$F$53</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1707,7 +1707,7 @@
             <c:noEndCap val="0"/>
             <c:plus>
               <c:numRef>
-                <c:f>Sheet1!$G$40:$G$44</c:f>
+                <c:f>Sheet1!$G$55:$G$59</c:f>
                 <c:numCache>
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="5"/>
@@ -1731,7 +1731,7 @@
             </c:plus>
             <c:minus>
               <c:numRef>
-                <c:f>Sheet1!$G$40:$G$44</c:f>
+                <c:f>Sheet1!$G$55:$G$59</c:f>
                 <c:numCache>
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="5"/>
@@ -1769,7 +1769,7 @@
           </c:errBars>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$B$40:$B$44</c:f>
+              <c:f>Sheet1!$B$55:$B$59</c:f>
               <c:strCache>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
@@ -1792,7 +1792,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$F$40:$F$44</c:f>
+              <c:f>Sheet1!$F$55:$F$59</c:f>
               <c:numCache>
                 <c:formatCode>0.0%</c:formatCode>
                 <c:ptCount val="5"/>
@@ -2119,7 +2119,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$C$38</c:f>
+              <c:f>Sheet1!$C$53</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -2140,7 +2140,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$B$73:$B$77</c:f>
+              <c:f>Sheet1!$B$88:$B$92</c:f>
               <c:strCache>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
@@ -2163,7 +2163,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$K$73:$K$77</c:f>
+              <c:f>Sheet1!$K$88:$K$92</c:f>
               <c:numCache>
                 <c:formatCode>0%</c:formatCode>
                 <c:ptCount val="5"/>
@@ -2196,7 +2196,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$F$38</c:f>
+              <c:f>Sheet1!$F$53</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -2217,7 +2217,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$B$73:$B$77</c:f>
+              <c:f>Sheet1!$B$88:$B$92</c:f>
               <c:strCache>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
@@ -2240,7 +2240,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$L$73:$L$77</c:f>
+              <c:f>Sheet1!$L$88:$L$92</c:f>
               <c:numCache>
                 <c:formatCode>0%</c:formatCode>
                 <c:ptCount val="5"/>
@@ -2565,7 +2565,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$C$38</c:f>
+              <c:f>Sheet1!$C$53</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -2586,7 +2586,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$B$73:$B$77</c:f>
+              <c:f>Sheet1!$B$88:$B$92</c:f>
               <c:strCache>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
@@ -2609,7 +2609,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$Q$73:$Q$77</c:f>
+              <c:f>Sheet1!$Q$88:$Q$92</c:f>
               <c:numCache>
                 <c:formatCode>#,##0</c:formatCode>
                 <c:ptCount val="5"/>
@@ -2642,7 +2642,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$F$38</c:f>
+              <c:f>Sheet1!$F$53</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -2663,7 +2663,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$B$73:$B$77</c:f>
+              <c:f>Sheet1!$B$88:$B$92</c:f>
               <c:strCache>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
@@ -2686,7 +2686,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$T$73:$T$77</c:f>
+              <c:f>Sheet1!$T$88:$T$92</c:f>
               <c:numCache>
                 <c:formatCode>_-* #,##0_-;\-* #,##0_-;_-* "-"??_-;_-@_-</c:formatCode>
                 <c:ptCount val="5"/>
@@ -3011,7 +3011,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$E$102</c:f>
+              <c:f>Sheet1!$E$117</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -3036,7 +3036,7 @@
             <c:noEndCap val="0"/>
             <c:plus>
               <c:numRef>
-                <c:f>Sheet1!$F$104:$F$107</c:f>
+                <c:f>Sheet1!$F$119:$F$122</c:f>
                 <c:numCache>
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="4"/>
@@ -3057,7 +3057,7 @@
             </c:plus>
             <c:minus>
               <c:numRef>
-                <c:f>Sheet1!$F$104:$F$107</c:f>
+                <c:f>Sheet1!$F$119:$F$122</c:f>
                 <c:numCache>
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="4"/>
@@ -3092,7 +3092,7 @@
           </c:errBars>
           <c:cat>
             <c:multiLvlStrRef>
-              <c:f>Sheet1!$C$104:$D$107</c:f>
+              <c:f>Sheet1!$C$119:$D$122</c:f>
               <c:multiLvlStrCache>
                 <c:ptCount val="4"/>
                 <c:lvl>
@@ -3122,7 +3122,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$E$104:$E$107</c:f>
+              <c:f>Sheet1!$E$119:$E$122</c:f>
               <c:numCache>
                 <c:formatCode>0.0%</c:formatCode>
                 <c:ptCount val="4"/>
@@ -3152,7 +3152,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$H$102</c:f>
+              <c:f>Sheet1!$H$117</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -3177,7 +3177,7 @@
             <c:noEndCap val="0"/>
             <c:plus>
               <c:numRef>
-                <c:f>Sheet1!$I$104:$I$107</c:f>
+                <c:f>Sheet1!$I$119:$I$122</c:f>
                 <c:numCache>
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="4"/>
@@ -3198,7 +3198,7 @@
             </c:plus>
             <c:minus>
               <c:numRef>
-                <c:f>Sheet1!$I$104:$I$107</c:f>
+                <c:f>Sheet1!$I$119:$I$122</c:f>
                 <c:numCache>
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="4"/>
@@ -3233,7 +3233,7 @@
           </c:errBars>
           <c:cat>
             <c:multiLvlStrRef>
-              <c:f>Sheet1!$C$104:$D$107</c:f>
+              <c:f>Sheet1!$C$119:$D$122</c:f>
               <c:multiLvlStrCache>
                 <c:ptCount val="4"/>
                 <c:lvl>
@@ -3263,7 +3263,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$H$104:$H$107</c:f>
+              <c:f>Sheet1!$H$119:$H$122</c:f>
               <c:numCache>
                 <c:formatCode>0.0%</c:formatCode>
                 <c:ptCount val="4"/>
@@ -3595,7 +3595,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$C$139</c:f>
+              <c:f>Sheet1!$C$154</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -3652,7 +3652,6 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable/>
-                  <c15:xForSave val="1"/>
                   <c15:showDataLabelsRange val="1"/>
                 </c:ext>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
@@ -3695,7 +3694,6 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable/>
-                  <c15:xForSave val="1"/>
                   <c15:showDataLabelsRange val="1"/>
                 </c:ext>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
@@ -3762,7 +3760,7 @@
           </c:dLbls>
           <c:cat>
             <c:multiLvlStrRef>
-              <c:f>Sheet1!$D$136:$G$137</c:f>
+              <c:f>Sheet1!$D$151:$G$152</c:f>
               <c:multiLvlStrCache>
                 <c:ptCount val="4"/>
                 <c:lvl>
@@ -3792,7 +3790,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$D$139:$G$139</c:f>
+              <c:f>Sheet1!$D$154:$G$154</c:f>
               <c:numCache>
                 <c:formatCode>_-* #,##0_-;\-* #,##0_-;_-* "-"??_-;_-@_-</c:formatCode>
                 <c:ptCount val="4"/>
@@ -3814,7 +3812,7 @@
           <c:extLst>
             <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
               <c15:datalabelsRange>
-                <c15:f>Sheet1!$I$139:$L$139</c15:f>
+                <c15:f>Sheet1!$I$154:$L$154</c15:f>
                 <c15:dlblRangeCache>
                   <c:ptCount val="4"/>
                   <c:pt idx="0">
@@ -3842,7 +3840,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$C$140</c:f>
+              <c:f>Sheet1!$C$155</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -3887,7 +3885,6 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable/>
-                  <c15:xForSave val="1"/>
                   <c15:showDataLabelsRange val="1"/>
                 </c:ext>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
@@ -3920,7 +3917,6 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable/>
-                  <c15:xForSave val="1"/>
                   <c15:showDataLabelsRange val="1"/>
                 </c:ext>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
@@ -3953,7 +3949,6 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable/>
-                  <c15:xForSave val="1"/>
                   <c15:showDataLabelsRange val="1"/>
                 </c:ext>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
@@ -3986,7 +3981,6 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable/>
-                  <c15:xForSave val="1"/>
                   <c15:showDataLabelsRange val="1"/>
                 </c:ext>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
@@ -4050,7 +4044,7 @@
           </c:dLbls>
           <c:cat>
             <c:multiLvlStrRef>
-              <c:f>Sheet1!$D$136:$G$137</c:f>
+              <c:f>Sheet1!$D$151:$G$152</c:f>
               <c:multiLvlStrCache>
                 <c:ptCount val="4"/>
                 <c:lvl>
@@ -4080,7 +4074,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$D$140:$G$140</c:f>
+              <c:f>Sheet1!$D$155:$G$155</c:f>
               <c:numCache>
                 <c:formatCode>_-* #,##0_-;\-* #,##0_-;_-* "-"??_-;_-@_-</c:formatCode>
                 <c:ptCount val="4"/>
@@ -4102,7 +4096,7 @@
           <c:extLst>
             <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
               <c15:datalabelsRange>
-                <c15:f>Sheet1!$I$140:$L$140</c15:f>
+                <c15:f>Sheet1!$I$155:$L$155</c15:f>
                 <c15:dlblRangeCache>
                   <c:ptCount val="4"/>
                   <c:pt idx="0">
@@ -4130,7 +4124,7 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$C$141</c:f>
+              <c:f>Sheet1!$C$156</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -4175,7 +4169,6 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable/>
-                  <c15:xForSave val="1"/>
                   <c15:showDataLabelsRange val="1"/>
                 </c:ext>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
@@ -4208,7 +4201,6 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable/>
-                  <c15:xForSave val="1"/>
                   <c15:showDataLabelsRange val="1"/>
                 </c:ext>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
@@ -4241,7 +4233,6 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable/>
-                  <c15:xForSave val="1"/>
                   <c15:showDataLabelsRange val="1"/>
                 </c:ext>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
@@ -4274,7 +4265,6 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable/>
-                  <c15:xForSave val="1"/>
                   <c15:showDataLabelsRange val="1"/>
                 </c:ext>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
@@ -4338,7 +4328,7 @@
           </c:dLbls>
           <c:cat>
             <c:multiLvlStrRef>
-              <c:f>Sheet1!$D$136:$G$137</c:f>
+              <c:f>Sheet1!$D$151:$G$152</c:f>
               <c:multiLvlStrCache>
                 <c:ptCount val="4"/>
                 <c:lvl>
@@ -4368,7 +4358,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$D$141:$G$141</c:f>
+              <c:f>Sheet1!$D$156:$G$156</c:f>
               <c:numCache>
                 <c:formatCode>_-* #,##0_-;\-* #,##0_-;_-* "-"??_-;_-@_-</c:formatCode>
                 <c:ptCount val="4"/>
@@ -4390,7 +4380,7 @@
           <c:extLst>
             <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
               <c15:datalabelsRange>
-                <c15:f>Sheet1!$I$141:$L$141</c15:f>
+                <c15:f>Sheet1!$I$156:$L$156</c15:f>
                 <c15:dlblRangeCache>
                   <c:ptCount val="4"/>
                   <c:pt idx="0">
@@ -4418,7 +4408,7 @@
           <c:order val="3"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$C$142</c:f>
+              <c:f>Sheet1!$C$157</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -4463,7 +4453,6 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable/>
-                  <c15:xForSave val="1"/>
                   <c15:showDataLabelsRange val="1"/>
                 </c:ext>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
@@ -4496,7 +4485,6 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable/>
-                  <c15:xForSave val="1"/>
                   <c15:showDataLabelsRange val="1"/>
                 </c:ext>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
@@ -4529,7 +4517,6 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable/>
-                  <c15:xForSave val="1"/>
                   <c15:showDataLabelsRange val="1"/>
                 </c:ext>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
@@ -4562,7 +4549,6 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable/>
-                  <c15:xForSave val="1"/>
                   <c15:showDataLabelsRange val="1"/>
                 </c:ext>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
@@ -4626,7 +4612,7 @@
           </c:dLbls>
           <c:cat>
             <c:multiLvlStrRef>
-              <c:f>Sheet1!$D$136:$G$137</c:f>
+              <c:f>Sheet1!$D$151:$G$152</c:f>
               <c:multiLvlStrCache>
                 <c:ptCount val="4"/>
                 <c:lvl>
@@ -4656,7 +4642,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$D$142:$G$142</c:f>
+              <c:f>Sheet1!$D$157:$G$157</c:f>
               <c:numCache>
                 <c:formatCode>_-* #,##0_-;\-* #,##0_-;_-* "-"??_-;_-@_-</c:formatCode>
                 <c:ptCount val="4"/>
@@ -4678,7 +4664,7 @@
           <c:extLst>
             <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
               <c15:datalabelsRange>
-                <c15:f>Sheet1!$I$142:$L$142</c15:f>
+                <c15:f>Sheet1!$I$157:$L$157</c15:f>
                 <c15:dlblRangeCache>
                   <c:ptCount val="4"/>
                   <c:pt idx="0">
@@ -4706,7 +4692,7 @@
           <c:order val="4"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$C$143</c:f>
+              <c:f>Sheet1!$C$158</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -4751,7 +4737,6 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable/>
-                  <c15:xForSave val="1"/>
                   <c15:showDataLabelsRange val="1"/>
                 </c:ext>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
@@ -4784,7 +4769,6 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable/>
-                  <c15:xForSave val="1"/>
                   <c15:showDataLabelsRange val="1"/>
                 </c:ext>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
@@ -4817,7 +4801,6 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable/>
-                  <c15:xForSave val="1"/>
                   <c15:showDataLabelsRange val="1"/>
                 </c:ext>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
@@ -4850,7 +4833,6 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable/>
-                  <c15:xForSave val="1"/>
                   <c15:showDataLabelsRange val="1"/>
                 </c:ext>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
@@ -4914,7 +4896,7 @@
           </c:dLbls>
           <c:cat>
             <c:multiLvlStrRef>
-              <c:f>Sheet1!$D$136:$G$137</c:f>
+              <c:f>Sheet1!$D$151:$G$152</c:f>
               <c:multiLvlStrCache>
                 <c:ptCount val="4"/>
                 <c:lvl>
@@ -4944,7 +4926,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$D$143:$G$143</c:f>
+              <c:f>Sheet1!$D$158:$G$158</c:f>
               <c:numCache>
                 <c:formatCode>_-* #,##0_-;\-* #,##0_-;_-* "-"??_-;_-@_-</c:formatCode>
                 <c:ptCount val="4"/>
@@ -4966,7 +4948,7 @@
           <c:extLst>
             <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
               <c15:datalabelsRange>
-                <c15:f>Sheet1!$I$143:$L$143</c15:f>
+                <c15:f>Sheet1!$I$158:$L$158</c15:f>
                 <c15:dlblRangeCache>
                   <c:ptCount val="4"/>
                   <c:pt idx="0">
@@ -8511,13 +8493,13 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>106361</xdr:colOff>
-      <xdr:row>45</xdr:row>
+      <xdr:row>60</xdr:row>
       <xdr:rowOff>144461</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
       <xdr:colOff>96837</xdr:colOff>
-      <xdr:row>66</xdr:row>
+      <xdr:row>81</xdr:row>
       <xdr:rowOff>106361</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -8547,13 +8529,13 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>78</xdr:row>
+      <xdr:row>93</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
       <xdr:colOff>635001</xdr:colOff>
-      <xdr:row>98</xdr:row>
+      <xdr:row>113</xdr:row>
       <xdr:rowOff>146050</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -8585,13 +8567,13 @@
     <xdr:from>
       <xdr:col>12</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>78</xdr:row>
+      <xdr:row>93</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>21</xdr:col>
       <xdr:colOff>90488</xdr:colOff>
-      <xdr:row>98</xdr:row>
+      <xdr:row>113</xdr:row>
       <xdr:rowOff>144462</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -8623,13 +8605,13 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>641350</xdr:colOff>
-      <xdr:row>109</xdr:row>
+      <xdr:row>124</xdr:row>
       <xdr:rowOff>57150</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
       <xdr:colOff>630238</xdr:colOff>
-      <xdr:row>130</xdr:row>
+      <xdr:row>145</xdr:row>
       <xdr:rowOff>17462</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -8661,13 +8643,13 @@
     <xdr:from>
       <xdr:col>5</xdr:col>
       <xdr:colOff>25400</xdr:colOff>
-      <xdr:row>120</xdr:row>
+      <xdr:row>135</xdr:row>
       <xdr:rowOff>165100</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
       <xdr:colOff>469900</xdr:colOff>
-      <xdr:row>125</xdr:row>
+      <xdr:row>140</xdr:row>
       <xdr:rowOff>133350</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -8727,17 +8709,17 @@
     <xdr:from>
       <xdr:col>2</xdr:col>
       <xdr:colOff>247200</xdr:colOff>
-      <xdr:row>113</xdr:row>
+      <xdr:row>128</xdr:row>
       <xdr:rowOff>87152</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
       <xdr:colOff>247560</xdr:colOff>
-      <xdr:row>113</xdr:row>
+      <xdr:row>128</xdr:row>
       <xdr:rowOff>90687</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId6">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="12" name="Ink 11">
@@ -8756,7 +8738,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="12" name="Ink 11">
@@ -8792,17 +8774,17 @@
     <xdr:from>
       <xdr:col>12</xdr:col>
       <xdr:colOff>634830</xdr:colOff>
-      <xdr:row>63</xdr:row>
+      <xdr:row>78</xdr:row>
       <xdr:rowOff>86160</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>643101</xdr:colOff>
-      <xdr:row>63</xdr:row>
+      <xdr:colOff>607509</xdr:colOff>
+      <xdr:row>78</xdr:row>
       <xdr:rowOff>90268</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId8">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="15" name="Ink 14">
@@ -8821,7 +8803,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="15" name="Ink 14">
@@ -8857,13 +8839,13 @@
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>145</xdr:row>
+      <xdr:row>160</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
       <xdr:colOff>638176</xdr:colOff>
-      <xdr:row>165</xdr:row>
+      <xdr:row>180</xdr:row>
       <xdr:rowOff>144462</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -9249,31 +9231,31 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B3:T143"/>
+  <dimension ref="B3:T158"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A60" workbookViewId="0">
-      <selection activeCell="X82" sqref="X82"/>
+    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
+      <selection activeCell="N32" sqref="N32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="8" max="8" width="10.46484375" customWidth="1"/>
-    <col min="12" max="12" width="12.19921875" customWidth="1"/>
-    <col min="15" max="15" width="10.1328125" customWidth="1"/>
-    <col min="17" max="17" width="9.9296875" customWidth="1"/>
+    <col min="8" max="8" width="10.42578125" customWidth="1"/>
+    <col min="12" max="12" width="12.140625" customWidth="1"/>
+    <col min="15" max="15" width="10.140625" customWidth="1"/>
+    <col min="17" max="17" width="10" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:17" x14ac:dyDescent="0.45">
+    <row r="3" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="2:17" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="5" spans="2:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="N5" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="6" spans="2:17" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="6" spans="2:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C6" s="1" t="s">
         <v>2</v>
       </c>
@@ -9289,7 +9271,7 @@
       <c r="K6" s="2"/>
       <c r="L6" s="3"/>
     </row>
-    <row r="7" spans="2:17" ht="57.4" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="7" spans="2:17" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B7" s="4"/>
       <c r="C7" s="5" t="s">
         <v>4</v>
@@ -9334,7 +9316,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="8" spans="2:17" x14ac:dyDescent="0.45">
+    <row r="8" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B8" s="11">
         <v>2018</v>
       </c>
@@ -9389,7 +9371,7 @@
         <v>1.6388814324532319E-2</v>
       </c>
     </row>
-    <row r="9" spans="2:17" x14ac:dyDescent="0.45">
+    <row r="9" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B9" s="17">
         <v>2019</v>
       </c>
@@ -9444,7 +9426,7 @@
         <v>1.7729728188980776E-2</v>
       </c>
     </row>
-    <row r="10" spans="2:17" x14ac:dyDescent="0.45">
+    <row r="10" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B10" s="17">
         <v>2020</v>
       </c>
@@ -9499,7 +9481,7 @@
         <v>2.1086051752421842E-2</v>
       </c>
     </row>
-    <row r="11" spans="2:17" x14ac:dyDescent="0.45">
+    <row r="11" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B11" s="17">
         <v>2021</v>
       </c>
@@ -9554,7 +9536,7 @@
         <v>2.0765963345535488E-2</v>
       </c>
     </row>
-    <row r="12" spans="2:17" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="12" spans="2:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B12" s="23">
         <v>2022</v>
       </c>
@@ -9609,94 +9591,286 @@
         <v>2.2535686420780854E-2</v>
       </c>
     </row>
-    <row r="35" spans="2:8" x14ac:dyDescent="0.45">
-      <c r="B35" t="s">
-        <v>0</v>
+    <row r="35" spans="2:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="36" spans="2:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C36" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D36" s="2"/>
+      <c r="E36" s="3"/>
+      <c r="G36" s="2"/>
+      <c r="H36" s="1" t="s">
+        <v>3</v>
       </c>
     </row>
-    <row r="37" spans="2:8" ht="14.65" thickBot="1" x14ac:dyDescent="0.5"/>
-    <row r="38" spans="2:8" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="C38" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D38" s="2"/>
-      <c r="E38" s="3"/>
-      <c r="F38" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="G38" s="2"/>
-      <c r="H38" s="3"/>
+    <row r="37" spans="2:17" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B37" s="4"/>
+      <c r="C37" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="D37" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="E37" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="F37" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="G37" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="H37" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="I37" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="J37" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="K37" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="L37" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="N37" s="29" t="s">
+        <v>10</v>
+      </c>
+      <c r="O37" s="29" t="s">
+        <v>11</v>
+      </c>
+      <c r="P37" s="29" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q37" s="29" t="s">
+        <v>12</v>
+      </c>
     </row>
-    <row r="39" spans="2:8" ht="57.4" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B39" s="4"/>
-      <c r="C39" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="D39" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="E39" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="F39" s="8" t="s">
-        <v>4</v>
-      </c>
-      <c r="G39" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="H39" s="10" t="s">
-        <v>6</v>
+    <row r="38" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B38" s="11">
+        <v>2018</v>
+      </c>
+      <c r="C38" s="12">
+        <v>0.68373984731547399</v>
+      </c>
+      <c r="D38" s="15">
+        <v>1.3030274609364E-2</v>
+      </c>
+      <c r="E38" s="15">
+        <f>C38+D38</f>
+        <v>0.696770121924838</v>
+      </c>
+      <c r="F38" s="15">
+        <f>C38-D38</f>
+        <v>0.67070957270610998</v>
+      </c>
+      <c r="G38" s="13">
+        <v>1147726</v>
+      </c>
+      <c r="H38" s="12">
+        <v>0.68203239181976605</v>
+      </c>
+      <c r="I38" s="15">
+        <v>1.11446599426694E-2</v>
+      </c>
+      <c r="J38" s="15">
+        <f>H38+I38</f>
+        <v>0.69317705176243549</v>
+      </c>
+      <c r="K38" s="15">
+        <f>H38-I38</f>
+        <v>0.6708877318770966</v>
+      </c>
+      <c r="L38" s="16">
+        <v>1847380</v>
+      </c>
+      <c r="N38" s="30">
+        <f>K38</f>
+        <v>0.6708877318770966</v>
+      </c>
+      <c r="O38" s="30">
+        <f>J38-K38</f>
+        <v>2.2289319885338887E-2</v>
+      </c>
+      <c r="P38" s="30">
+        <f>F38-J38</f>
+        <v>-2.2467479056325512E-2</v>
+      </c>
+      <c r="Q38" s="30">
+        <f>E38-F38</f>
+        <v>2.6060549218728024E-2</v>
       </c>
     </row>
-    <row r="40" spans="2:8" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B40" s="23" t="s">
-        <v>14</v>
-      </c>
-      <c r="C40" s="24">
-        <v>0.79933259145512303</v>
-      </c>
-      <c r="D40" s="25">
-        <v>1.1267843210390399E-2</v>
-      </c>
-      <c r="E40" s="26">
-        <v>2128831</v>
-      </c>
-      <c r="F40" s="27">
-        <v>0.712854868118178</v>
-      </c>
-      <c r="G40" s="25">
-        <v>1.03687839954644E-2</v>
-      </c>
-      <c r="H40" s="28">
-        <v>4121038</v>
+    <row r="39" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B39" s="17">
+        <v>2019</v>
+      </c>
+      <c r="C39" s="18">
+        <v>0.68876877637130796</v>
+      </c>
+      <c r="D39" s="19">
+        <v>1.3428488741999201E-2</v>
+      </c>
+      <c r="E39" s="19">
+        <f t="shared" ref="E39:E42" si="8">C39+D39</f>
+        <v>0.70219726511330716</v>
+      </c>
+      <c r="F39" s="19">
+        <f t="shared" ref="F39:F42" si="9">C39-D39</f>
+        <v>0.67534028762930876</v>
+      </c>
+      <c r="G39" s="20">
+        <v>1185000</v>
+      </c>
+      <c r="H39" s="18">
+        <v>0.68767282696699705</v>
+      </c>
+      <c r="I39" s="19">
+        <v>1.13776465862128E-2</v>
+      </c>
+      <c r="J39" s="19">
+        <f t="shared" ref="J39:J42" si="10">H39+I39</f>
+        <v>0.69905047355320982</v>
+      </c>
+      <c r="K39" s="19">
+        <f t="shared" ref="K39:K42" si="11">H39-I39</f>
+        <v>0.67629518038078429</v>
+      </c>
+      <c r="L39" s="22">
+        <v>1861327</v>
+      </c>
+      <c r="N39" s="30">
+        <f t="shared" ref="N39:N42" si="12">K39</f>
+        <v>0.67629518038078429</v>
+      </c>
+      <c r="O39" s="30">
+        <f t="shared" ref="O39:O42" si="13">J39-K39</f>
+        <v>2.2755293172425528E-2</v>
+      </c>
+      <c r="P39" s="30">
+        <f t="shared" ref="P39:P42" si="14">F39-J39</f>
+        <v>-2.3710185923901061E-2</v>
+      </c>
+      <c r="Q39" s="30">
+        <f t="shared" ref="Q39:Q42" si="15">E39-F39</f>
+        <v>2.6856977483998401E-2</v>
       </c>
     </row>
-    <row r="41" spans="2:8" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B41" s="23" t="s">
-        <v>15</v>
-      </c>
-      <c r="C41" s="24">
-        <v>0.92668473911135196</v>
-      </c>
-      <c r="D41" s="25">
-        <v>1.05909783386849E-2</v>
-      </c>
-      <c r="E41" s="26">
-        <v>968325</v>
-      </c>
-      <c r="F41" s="27">
-        <v>0.72742104358135695</v>
-      </c>
-      <c r="G41" s="25">
-        <v>1.3783532832492101E-2</v>
-      </c>
-      <c r="H41" s="28">
-        <v>2157551</v>
+    <row r="40" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B40" s="17">
+        <v>2020</v>
+      </c>
+      <c r="C40" s="18">
+        <v>0.69507634591029699</v>
+      </c>
+      <c r="D40" s="19">
+        <v>1.6169859205193898E-2</v>
+      </c>
+      <c r="E40" s="19">
+        <f t="shared" si="8"/>
+        <v>0.71124620511549086</v>
+      </c>
+      <c r="F40" s="19">
+        <f t="shared" si="9"/>
+        <v>0.67890648670510312</v>
+      </c>
+      <c r="G40" s="20">
+        <v>1171772</v>
+      </c>
+      <c r="H40" s="18">
+        <v>0.70641098894904497</v>
+      </c>
+      <c r="I40" s="19">
+        <v>1.4645902095903499E-2</v>
+      </c>
+      <c r="J40" s="19">
+        <f t="shared" si="10"/>
+        <v>0.72105689104494852</v>
+      </c>
+      <c r="K40" s="19">
+        <f t="shared" si="11"/>
+        <v>0.69176508685314142</v>
+      </c>
+      <c r="L40" s="22">
+        <v>1951415</v>
+      </c>
+      <c r="N40" s="30">
+        <f t="shared" si="12"/>
+        <v>0.69176508685314142</v>
+      </c>
+      <c r="O40" s="30">
+        <f t="shared" si="13"/>
+        <v>2.9291804191807103E-2</v>
+      </c>
+      <c r="P40" s="30">
+        <f t="shared" si="14"/>
+        <v>-4.2150404339845404E-2</v>
+      </c>
+      <c r="Q40" s="30">
+        <f t="shared" si="15"/>
+        <v>3.2339718410387741E-2</v>
       </c>
     </row>
-    <row r="42" spans="2:8" x14ac:dyDescent="0.45">
-      <c r="B42" s="31" t="s">
-        <v>16</v>
+    <row r="41" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B41" s="17">
+        <v>2021</v>
+      </c>
+      <c r="C41" s="18">
+        <v>0.70237208060949297</v>
+      </c>
+      <c r="D41" s="19">
+        <v>1.6355205575461398E-2</v>
+      </c>
+      <c r="E41" s="19">
+        <f t="shared" si="8"/>
+        <v>0.71872728618495441</v>
+      </c>
+      <c r="F41" s="19">
+        <f t="shared" si="9"/>
+        <v>0.68601687503403153</v>
+      </c>
+      <c r="G41" s="20">
+        <v>1154008</v>
+      </c>
+      <c r="H41" s="18">
+        <v>0.70862683351288602</v>
+      </c>
+      <c r="I41" s="19">
+        <v>1.21421072255011E-2</v>
+      </c>
+      <c r="J41" s="19">
+        <f t="shared" si="10"/>
+        <v>0.72076894073838715</v>
+      </c>
+      <c r="K41" s="19">
+        <f t="shared" si="11"/>
+        <v>0.69648472628738489</v>
+      </c>
+      <c r="L41" s="22">
+        <v>1930720</v>
+      </c>
+      <c r="N41" s="30">
+        <f t="shared" si="12"/>
+        <v>0.69648472628738489</v>
+      </c>
+      <c r="O41" s="30">
+        <f t="shared" si="13"/>
+        <v>2.4284214451002262E-2</v>
+      </c>
+      <c r="P41" s="30">
+        <f t="shared" si="14"/>
+        <v>-3.4752065704355628E-2</v>
+      </c>
+      <c r="Q41" s="30">
+        <f t="shared" si="15"/>
+        <v>3.271041115092288E-2</v>
+      </c>
+    </row>
+    <row r="42" spans="2:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B42" s="31">
+        <v>2022</v>
       </c>
       <c r="C42" s="32">
         <v>0.69307009183924895</v>
@@ -9704,801 +9878,946 @@
       <c r="D42" s="33">
         <v>1.73185149047532E-2</v>
       </c>
-      <c r="E42" s="34">
+      <c r="E42" s="25">
+        <f t="shared" si="8"/>
+        <v>0.71038860674400217</v>
+      </c>
+      <c r="F42" s="25">
+        <f t="shared" si="9"/>
+        <v>0.67575157693449572</v>
+      </c>
+      <c r="G42" s="34">
         <v>1160506</v>
       </c>
-      <c r="F42" s="32">
+      <c r="H42" s="32">
         <v>0.69684902421049899</v>
       </c>
-      <c r="G42" s="33">
+      <c r="I42" s="33">
         <v>1.4223407773721899E-2</v>
       </c>
-      <c r="H42" s="35">
+      <c r="J42" s="25">
+        <f t="shared" si="10"/>
+        <v>0.71107243198422088</v>
+      </c>
+      <c r="K42" s="25">
+        <f t="shared" si="11"/>
+        <v>0.68262561643677711</v>
+      </c>
+      <c r="L42" s="35">
         <v>1963487</v>
       </c>
+      <c r="N42" s="30">
+        <f t="shared" si="12"/>
+        <v>0.68262561643677711</v>
+      </c>
+      <c r="O42" s="30">
+        <f t="shared" si="13"/>
+        <v>2.8446815547443771E-2</v>
+      </c>
+      <c r="P42" s="30">
+        <f t="shared" si="14"/>
+        <v>-3.5320855049725153E-2</v>
+      </c>
+      <c r="Q42" s="30">
+        <f t="shared" si="15"/>
+        <v>3.4637029809506448E-2</v>
+      </c>
     </row>
-    <row r="43" spans="2:8" x14ac:dyDescent="0.45">
-      <c r="B43" s="31" t="s">
+    <row r="50" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B50" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="53" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C53" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D53" s="2"/>
+      <c r="E53" s="3"/>
+      <c r="F53" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="G53" s="2"/>
+      <c r="H53" s="3"/>
+    </row>
+    <row r="54" spans="2:8" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B54" s="4"/>
+      <c r="C54" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="D54" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="E54" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="F54" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="G54" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="H54" s="10" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="55" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B55" s="23" t="s">
+        <v>14</v>
+      </c>
+      <c r="C55" s="24">
+        <v>0.79933259145512303</v>
+      </c>
+      <c r="D55" s="25">
+        <v>1.1267843210390399E-2</v>
+      </c>
+      <c r="E55" s="26">
+        <v>2128831</v>
+      </c>
+      <c r="F55" s="27">
+        <v>0.712854868118178</v>
+      </c>
+      <c r="G55" s="25">
+        <v>1.03687839954644E-2</v>
+      </c>
+      <c r="H55" s="28">
+        <v>4121038</v>
+      </c>
+    </row>
+    <row r="56" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B56" s="23" t="s">
+        <v>15</v>
+      </c>
+      <c r="C56" s="24">
+        <v>0.92668473911135196</v>
+      </c>
+      <c r="D56" s="25">
+        <v>1.05909783386849E-2</v>
+      </c>
+      <c r="E56" s="26">
+        <v>968325</v>
+      </c>
+      <c r="F56" s="27">
+        <v>0.72742104358135695</v>
+      </c>
+      <c r="G56" s="25">
+        <v>1.3783532832492101E-2</v>
+      </c>
+      <c r="H56" s="28">
+        <v>2157551</v>
+      </c>
+    </row>
+    <row r="57" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B57" s="31" t="s">
+        <v>16</v>
+      </c>
+      <c r="C57" s="32">
+        <v>0.69307009183924895</v>
+      </c>
+      <c r="D57" s="33">
+        <v>1.73185149047532E-2</v>
+      </c>
+      <c r="E57" s="34">
+        <v>1160506</v>
+      </c>
+      <c r="F57" s="32">
+        <v>0.69684902421049899</v>
+      </c>
+      <c r="G57" s="33">
+        <v>1.4223407773721899E-2</v>
+      </c>
+      <c r="H57" s="35">
+        <v>1963487</v>
+      </c>
+    </row>
+    <row r="58" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B58" s="31" t="s">
         <v>17</v>
       </c>
-      <c r="C43" s="32">
+      <c r="C58" s="32">
         <v>0.84620568430829102</v>
       </c>
-      <c r="D43" s="33">
+      <c r="D58" s="33">
         <v>1.36186819696885E-2</v>
       </c>
-      <c r="E43" s="34">
+      <c r="E58" s="34">
         <v>1102544</v>
       </c>
-      <c r="F43" s="32">
+      <c r="F58" s="32">
         <v>0.76244388299010402</v>
       </c>
-      <c r="G43" s="33">
+      <c r="G58" s="33">
         <v>1.2150622865273601E-2</v>
       </c>
-      <c r="H43" s="35">
+      <c r="H58" s="35">
         <v>2149972</v>
       </c>
     </row>
-    <row r="44" spans="2:8" x14ac:dyDescent="0.45">
-      <c r="B44" s="31" t="s">
+    <row r="59" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B59" s="31" t="s">
         <v>18</v>
       </c>
-      <c r="C44" s="32">
+      <c r="C59" s="32">
         <v>0.72710600508254997</v>
       </c>
-      <c r="D44" s="33">
+      <c r="D59" s="33">
         <v>1.8830962783656601E-2</v>
       </c>
-      <c r="E44" s="34">
+      <c r="E59" s="34">
         <v>899155</v>
       </c>
-      <c r="F44" s="32">
+      <c r="F59" s="32">
         <v>0.633415987774545</v>
       </c>
-      <c r="G44" s="33">
+      <c r="G59" s="33">
         <v>2.0722296241639598E-2</v>
       </c>
-      <c r="H44" s="35">
+      <c r="H59" s="35">
         <v>1296966</v>
       </c>
     </row>
-    <row r="69" spans="2:20" x14ac:dyDescent="0.45">
-      <c r="B69" t="s">
+    <row r="84" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B84" t="s">
         <v>19</v>
       </c>
-      <c r="O69" t="s">
+      <c r="O84" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="70" spans="2:20" ht="14.65" thickBot="1" x14ac:dyDescent="0.5"/>
-    <row r="71" spans="2:20" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="D71" s="1" t="s">
+    <row r="85" spans="2:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="86" spans="2:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D86" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E71" s="2"/>
-      <c r="F71" s="3"/>
-      <c r="G71" s="1" t="s">
+      <c r="E86" s="2"/>
+      <c r="F86" s="3"/>
+      <c r="G86" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="H71" s="2"/>
-      <c r="I71" s="3"/>
-      <c r="O71" s="1" t="s">
+      <c r="H86" s="2"/>
+      <c r="I86" s="3"/>
+      <c r="O86" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="P71" s="2"/>
-      <c r="Q71" s="3"/>
-      <c r="R71" s="1" t="s">
+      <c r="P86" s="2"/>
+      <c r="Q86" s="3"/>
+      <c r="R86" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="S71" s="2"/>
-      <c r="T71" s="3"/>
+      <c r="S86" s="2"/>
+      <c r="T86" s="3"/>
     </row>
-    <row r="72" spans="2:20" ht="57.4" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B72" s="36"/>
-      <c r="C72" s="4"/>
-      <c r="D72" s="5" t="s">
+    <row r="87" spans="2:20" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B87" s="36"/>
+      <c r="C87" s="4"/>
+      <c r="D87" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="E72" s="6" t="s">
+      <c r="E87" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="F72" s="7" t="s">
+      <c r="F87" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="G72" s="8" t="s">
+      <c r="G87" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="H72" s="9" t="s">
+      <c r="H87" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="I72" s="10" t="s">
+      <c r="I87" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="O72" s="5" t="s">
+      <c r="O87" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="P72" s="6" t="s">
+      <c r="P87" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="Q72" s="7" t="s">
+      <c r="Q87" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="R72" s="8" t="s">
+      <c r="R87" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="S72" s="9" t="s">
+      <c r="S87" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="T72" s="10" t="s">
+      <c r="T87" s="10" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="73" spans="2:20" ht="28.9" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B73" s="37" t="s">
+    <row r="88" spans="2:20" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B88" s="37" t="s">
         <v>20</v>
       </c>
-      <c r="C73" s="23">
+      <c r="C88" s="23">
         <v>2022</v>
       </c>
-      <c r="D73" s="24">
+      <c r="D88" s="24">
         <v>0</v>
       </c>
-      <c r="E73" s="25">
+      <c r="E88" s="25">
         <v>0</v>
       </c>
-      <c r="F73" s="26">
+      <c r="F88" s="26">
         <v>2848</v>
       </c>
-      <c r="G73" s="27">
+      <c r="G88" s="27">
         <v>0.156390149230245</v>
       </c>
-      <c r="H73" s="25">
+      <c r="H88" s="25">
         <v>3.4288647309644198E-2</v>
       </c>
-      <c r="I73" s="28">
+      <c r="I88" s="28">
         <v>228774</v>
       </c>
-      <c r="K73" s="67">
-        <f>F73/SUM(F$73:F$77)</f>
+      <c r="K88" s="65">
+        <f>F88/SUM(F$88:F$92)</f>
         <v>1.337823434551639E-3</v>
       </c>
-      <c r="L73" s="67">
-        <f>G73/SUM(G$73:G$77)</f>
+      <c r="L88" s="65">
+        <f>G88/SUM(G$88:G$92)</f>
         <v>5.0123086443735511E-2</v>
       </c>
-      <c r="O73" s="24">
+      <c r="O88" s="24">
         <v>0</v>
       </c>
-      <c r="P73" s="25">
+      <c r="P88" s="25">
         <v>0</v>
       </c>
-      <c r="Q73" s="26">
+      <c r="Q88" s="26">
         <v>4073</v>
       </c>
-      <c r="R73" s="27">
+      <c r="R88" s="27">
         <v>0.22753347912538499</v>
       </c>
-      <c r="S73" s="25">
+      <c r="S88" s="25">
         <v>1.12995254747055E-2</v>
       </c>
-      <c r="T73" s="28">
+      <c r="T88" s="28">
         <v>1460985</v>
       </c>
     </row>
-    <row r="74" spans="2:20" ht="28.9" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B74" s="37" t="s">
+    <row r="89" spans="2:20" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B89" s="37" t="s">
         <v>21</v>
       </c>
-      <c r="C74" s="31">
+      <c r="C89" s="31">
         <v>2022</v>
       </c>
-      <c r="D74" s="32">
+      <c r="D89" s="32">
         <v>0.37879936010777099</v>
       </c>
-      <c r="E74" s="33">
+      <c r="E89" s="33">
         <v>0.17094868918207601</v>
       </c>
-      <c r="F74" s="34">
+      <c r="F89" s="34">
         <v>23754</v>
       </c>
-      <c r="G74" s="32">
+      <c r="G89" s="32">
         <v>0.53690713703835602</v>
       </c>
-      <c r="H74" s="33">
+      <c r="H89" s="33">
         <v>2.5545960711472599E-2</v>
       </c>
-      <c r="I74" s="35">
+      <c r="I89" s="35">
         <v>820004</v>
       </c>
-      <c r="K74" s="67">
-        <f t="shared" ref="K74:L77" si="8">F74/SUM(F$73:F$77)</f>
+      <c r="K89" s="65">
+        <f t="shared" ref="K89:L92" si="16">F89/SUM(F$88:F$92)</f>
         <v>1.1158236609669815E-2</v>
       </c>
-      <c r="L74" s="67">
-        <f t="shared" si="8"/>
+      <c r="L89" s="65">
+        <f t="shared" si="16"/>
         <v>0.17207888715811484</v>
       </c>
-      <c r="O74" s="32">
+      <c r="O89" s="32">
         <v>0.57470227417596398</v>
       </c>
-      <c r="P74" s="33">
+      <c r="P89" s="33">
         <v>5.5550415155696697E-2</v>
       </c>
-      <c r="Q74" s="34">
+      <c r="Q89" s="34">
         <v>287093</v>
       </c>
-      <c r="R74" s="32">
+      <c r="R89" s="32">
         <v>0.60569152688973105</v>
       </c>
-      <c r="S74" s="33">
+      <c r="S89" s="33">
         <v>1.18356916561004E-2</v>
       </c>
-      <c r="T74" s="35">
+      <c r="T89" s="35">
         <v>5068552</v>
       </c>
     </row>
-    <row r="75" spans="2:20" ht="28.9" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B75" s="38" t="s">
+    <row r="90" spans="2:20" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B90" s="38" t="s">
         <v>22</v>
       </c>
-      <c r="C75" s="23">
+      <c r="C90" s="23">
         <v>2022</v>
       </c>
-      <c r="D75" s="24">
+      <c r="D90" s="24">
         <v>0.654116853960381</v>
       </c>
-      <c r="E75" s="25">
+      <c r="E90" s="25">
         <v>3.7122932812727799E-2</v>
       </c>
-      <c r="F75" s="26">
+      <c r="F90" s="26">
         <v>323378</v>
       </c>
-      <c r="G75" s="24">
+      <c r="G90" s="24">
         <v>0.86072573995033597</v>
       </c>
-      <c r="H75" s="25">
+      <c r="H90" s="25">
         <v>1.49910933603542E-2</v>
       </c>
-      <c r="I75" s="28">
+      <c r="I90" s="28">
         <v>1281809</v>
       </c>
-      <c r="K75" s="67">
-        <f t="shared" si="8"/>
+      <c r="K90" s="65">
+        <f t="shared" si="16"/>
         <v>0.15190402620029492</v>
       </c>
-      <c r="L75" s="67">
-        <f t="shared" si="8"/>
+      <c r="L90" s="65">
+        <f t="shared" si="16"/>
         <v>0.27586283970074654</v>
       </c>
-      <c r="O75" s="24">
+      <c r="O90" s="24">
         <v>0.77785784199696095</v>
       </c>
-      <c r="P75" s="25">
+      <c r="P90" s="25">
         <v>9.2520544076411804E-3</v>
       </c>
-      <c r="Q75" s="26">
+      <c r="Q90" s="26">
         <v>3125269</v>
       </c>
-      <c r="R75" s="24">
+      <c r="R90" s="24">
         <v>0.86854392893506704</v>
       </c>
-      <c r="S75" s="25">
+      <c r="S90" s="25">
         <v>5.9153296508353903E-3</v>
       </c>
-      <c r="T75" s="28">
+      <c r="T90" s="28">
         <v>5791661</v>
       </c>
     </row>
-    <row r="76" spans="2:20" ht="28.9" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B76" s="37" t="s">
+    <row r="91" spans="2:20" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B91" s="37" t="s">
         <v>23</v>
       </c>
-      <c r="C76" s="23">
+      <c r="C91" s="23">
         <v>2022</v>
       </c>
-      <c r="D76" s="24">
+      <c r="D91" s="24">
         <v>0.83550437368352204</v>
       </c>
-      <c r="E76" s="25">
+      <c r="E91" s="25">
         <v>1.24987517244406E-2</v>
       </c>
-      <c r="F76" s="26">
+      <c r="F91" s="26">
         <v>1360638</v>
       </c>
-      <c r="G76" s="24">
+      <c r="G91" s="24">
         <v>0.88510018182858796</v>
       </c>
-      <c r="H76" s="25">
+      <c r="H91" s="25">
         <v>1.4664451939298301E-2</v>
       </c>
-      <c r="I76" s="28">
+      <c r="I91" s="28">
         <v>681411</v>
       </c>
-      <c r="K76" s="67">
-        <f t="shared" si="8"/>
+      <c r="K91" s="65">
+        <f t="shared" si="16"/>
         <v>0.63914796430529242</v>
       </c>
-      <c r="L76" s="67">
-        <f t="shared" si="8"/>
+      <c r="L91" s="65">
+        <f t="shared" si="16"/>
         <v>0.28367485512048218</v>
       </c>
-      <c r="O76" s="24">
+      <c r="O91" s="24">
         <v>0.858524078476263</v>
       </c>
-      <c r="P76" s="25">
+      <c r="P91" s="25">
         <v>4.2611303298503399E-3</v>
       </c>
-      <c r="Q76" s="26">
+      <c r="Q91" s="26">
         <v>8547094</v>
       </c>
-      <c r="R76" s="24">
+      <c r="R91" s="24">
         <v>0.85049191070230301</v>
       </c>
-      <c r="S76" s="25">
+      <c r="S91" s="25">
         <v>5.9803404560759997E-3</v>
       </c>
-      <c r="T76" s="28">
+      <c r="T91" s="28">
         <v>4132559</v>
       </c>
     </row>
-    <row r="77" spans="2:20" ht="28.9" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B77" s="37" t="s">
+    <row r="92" spans="2:20" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B92" s="37" t="s">
         <v>24</v>
       </c>
-      <c r="C77" s="23">
+      <c r="C92" s="23">
         <v>2022</v>
       </c>
-      <c r="D77" s="24">
+      <c r="D92" s="24">
         <v>0.82326470004519203</v>
       </c>
-      <c r="E77" s="25">
+      <c r="E92" s="25">
         <v>2.22209055706417E-2</v>
       </c>
-      <c r="F77" s="26">
+      <c r="F92" s="26">
         <v>418213</v>
       </c>
-      <c r="G77" s="24">
+      <c r="G92" s="24">
         <v>0.68099888191589097</v>
       </c>
-      <c r="H77" s="25">
+      <c r="H92" s="25">
         <v>1.6739280203586698E-2</v>
       </c>
-      <c r="I77" s="28">
+      <c r="I92" s="28">
         <v>1109040</v>
       </c>
-      <c r="K77" s="67">
-        <f t="shared" si="8"/>
+      <c r="K92" s="65">
+        <f t="shared" si="16"/>
         <v>0.1964519494501912</v>
       </c>
-      <c r="L77" s="67">
-        <f t="shared" si="8"/>
+      <c r="L92" s="65">
+        <f t="shared" si="16"/>
         <v>0.21826033157692104</v>
       </c>
-      <c r="O77" s="24">
+      <c r="O92" s="24">
         <v>0.84478242876434095</v>
       </c>
-      <c r="P77" s="25">
+      <c r="P92" s="25">
         <v>7.8864302504463597E-3</v>
       </c>
-      <c r="Q77" s="26">
+      <c r="Q92" s="26">
         <v>2498538</v>
       </c>
-      <c r="R77" s="24">
+      <c r="R92" s="24">
         <v>0.68373064990839905</v>
       </c>
-      <c r="S77" s="25">
+      <c r="S92" s="25">
         <v>4.4157094066778497E-3</v>
       </c>
-      <c r="T77" s="28">
+      <c r="T92" s="28">
         <v>10554472</v>
       </c>
     </row>
-    <row r="101" spans="3:10" ht="14.65" thickBot="1" x14ac:dyDescent="0.5"/>
-    <row r="102" spans="3:10" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="E102" s="1" t="s">
+    <row r="116" spans="3:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="117" spans="3:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E117" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="F102" s="2"/>
-      <c r="G102" s="3"/>
-      <c r="H102" s="1" t="s">
+      <c r="F117" s="2"/>
+      <c r="G117" s="3"/>
+      <c r="H117" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="I102" s="2"/>
-      <c r="J102" s="3"/>
+      <c r="I117" s="2"/>
+      <c r="J117" s="3"/>
     </row>
-    <row r="103" spans="3:10" ht="57.4" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="D103" s="4"/>
-      <c r="E103" s="5" t="s">
+    <row r="118" spans="3:10" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D118" s="4"/>
+      <c r="E118" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="F103" s="6" t="s">
+      <c r="F118" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="G103" s="7" t="s">
+      <c r="G118" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="H103" s="8" t="s">
+      <c r="H118" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="I103" s="9" t="s">
+      <c r="I118" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="J103" s="10" t="s">
+      <c r="J118" s="10" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="104" spans="3:10" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="C104" s="39" t="s">
+    <row r="119" spans="3:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C119" s="67" t="s">
         <v>2</v>
       </c>
-      <c r="D104" s="23" t="s">
+      <c r="D119" s="23" t="s">
         <v>15</v>
       </c>
-      <c r="E104" s="24">
+      <c r="E119" s="24">
         <v>0.92668473911135196</v>
       </c>
-      <c r="F104" s="25">
+      <c r="F119" s="25">
         <v>1.05909783386849E-2</v>
       </c>
-      <c r="G104" s="26">
+      <c r="G119" s="26">
         <v>968325</v>
       </c>
-      <c r="H104" s="46">
+      <c r="H119" s="45">
         <v>0.92779677610091504</v>
       </c>
-      <c r="I104" s="48">
+      <c r="I119" s="47">
         <v>3.6682658956604798E-3</v>
       </c>
-      <c r="J104" s="47">
+      <c r="J119" s="46">
         <v>6484198</v>
       </c>
     </row>
-    <row r="105" spans="3:10" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="C105" s="39"/>
-      <c r="D105" s="23" t="s">
+    <row r="120" spans="3:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C120" s="67"/>
+      <c r="D120" s="23" t="s">
         <v>16</v>
       </c>
-      <c r="E105" s="24">
+      <c r="E120" s="24">
         <v>0.69307009183924895</v>
       </c>
-      <c r="F105" s="25">
+      <c r="F120" s="25">
         <v>1.73185149047532E-2</v>
       </c>
-      <c r="G105" s="26">
+      <c r="G120" s="26">
         <v>1160506</v>
       </c>
-      <c r="H105" s="52">
+      <c r="H120" s="51">
         <v>0.75566507798009697</v>
       </c>
-      <c r="I105" s="53">
+      <c r="I120" s="52">
         <v>5.4472118452649296E-3</v>
       </c>
-      <c r="J105" s="54">
+      <c r="J120" s="53">
         <v>7977869</v>
       </c>
     </row>
-    <row r="106" spans="3:10" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="C106" s="39" t="s">
+    <row r="121" spans="3:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C121" s="67" t="s">
         <v>3</v>
       </c>
-      <c r="D106" s="31" t="s">
+      <c r="D121" s="31" t="s">
         <v>15</v>
       </c>
-      <c r="E106" s="40">
+      <c r="E121" s="39">
         <v>0.72742104358135695</v>
       </c>
-      <c r="F106" s="42">
+      <c r="F121" s="41">
         <v>1.3783532832492101E-2</v>
       </c>
-      <c r="G106" s="41">
+      <c r="G121" s="40">
         <v>2157551</v>
       </c>
-      <c r="H106" s="50">
+      <c r="H121" s="49">
         <v>0.72201975027028897</v>
       </c>
-      <c r="I106" s="51">
+      <c r="I121" s="50">
         <v>5.3424684010458098E-3</v>
       </c>
-      <c r="J106" s="49">
+      <c r="J121" s="48">
         <v>14163553</v>
       </c>
     </row>
-    <row r="107" spans="3:10" x14ac:dyDescent="0.45">
-      <c r="C107" s="39"/>
-      <c r="D107" s="31" t="s">
+    <row r="122" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C122" s="67"/>
+      <c r="D122" s="31" t="s">
         <v>16</v>
       </c>
-      <c r="E107" s="43">
+      <c r="E122" s="42">
         <v>0.69684902421049899</v>
       </c>
-      <c r="F107" s="44">
+      <c r="F122" s="43">
         <v>1.4223407773721899E-2</v>
       </c>
-      <c r="G107" s="45">
+      <c r="G122" s="44">
         <v>1963487</v>
       </c>
-      <c r="H107" s="55">
+      <c r="H122" s="54">
         <v>0.695811478623517</v>
       </c>
-      <c r="I107" s="56">
+      <c r="I122" s="55">
         <v>4.4586455593805798E-3</v>
       </c>
-      <c r="J107" s="57">
+      <c r="J122" s="56">
         <v>12844676</v>
       </c>
     </row>
-    <row r="133" spans="3:12" x14ac:dyDescent="0.45">
-      <c r="C133" t="s">
+    <row r="148" spans="3:12" x14ac:dyDescent="0.25">
+      <c r="C148" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="135" spans="3:12" x14ac:dyDescent="0.45">
-      <c r="E135" t="s">
+    <row r="150" spans="3:12" x14ac:dyDescent="0.25">
+      <c r="E150" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="136" spans="3:12" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="D136" s="65" t="s">
+    <row r="151" spans="3:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D151" s="66" t="s">
         <v>27</v>
       </c>
-      <c r="E136" s="65"/>
-      <c r="F136" s="65" t="s">
+      <c r="E151" s="66"/>
+      <c r="F151" s="66" t="s">
         <v>26</v>
       </c>
-      <c r="G136" s="65"/>
-      <c r="H136" s="66"/>
-      <c r="I136" s="66"/>
+      <c r="G151" s="66"/>
+      <c r="H151" s="64"/>
+      <c r="I151" s="64"/>
     </row>
-    <row r="137" spans="3:12" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="D137" s="1" t="s">
+    <row r="152" spans="3:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D152" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E137" s="59" t="s">
+      <c r="E152" s="58" t="s">
         <v>3</v>
       </c>
-      <c r="F137" s="1" t="s">
+      <c r="F152" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="G137" s="59" t="s">
+      <c r="G152" s="58" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="138" spans="3:12" ht="57.4" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="C138" s="36"/>
-      <c r="D138" s="7" t="s">
+    <row r="153" spans="3:12" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C153" s="36"/>
+      <c r="D153" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="E138" s="10" t="s">
+      <c r="E153" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="F138" s="58" t="s">
+      <c r="F153" s="57" t="s">
         <v>6</v>
       </c>
-      <c r="G138" s="61" t="s">
+      <c r="G153" s="60" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="139" spans="3:12" ht="28.9" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="C139" s="37" t="s">
+    <row r="154" spans="3:12" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C154" s="37" t="s">
         <v>28</v>
       </c>
-      <c r="D139" s="34">
+      <c r="D154" s="34">
         <v>1181</v>
       </c>
-      <c r="E139" s="35">
+      <c r="E154" s="35">
         <v>127791</v>
       </c>
-      <c r="F139" s="64">
+      <c r="F154" s="63">
         <v>2406</v>
       </c>
-      <c r="G139" s="63">
+      <c r="G154" s="62">
         <v>713128</v>
       </c>
-      <c r="I139" s="67">
-        <f>D139/SUM(D$139:D$143)</f>
+      <c r="I154" s="65">
+        <f>D154/SUM(D$154:D$158)</f>
         <v>1.0176595381669719E-3</v>
       </c>
-      <c r="J139" s="67">
-        <f t="shared" ref="J139:L143" si="9">E139/SUM(E$139:E$143)</f>
+      <c r="J154" s="65">
+        <f t="shared" ref="J154:L158" si="17">E154/SUM(E$154:E$158)</f>
         <v>6.5083700579632059E-2</v>
       </c>
-      <c r="K139" s="67">
-        <f t="shared" si="9"/>
+      <c r="K154" s="65">
+        <f t="shared" si="17"/>
         <v>3.0158429525478544E-4</v>
       </c>
-      <c r="L139" s="67">
-        <f t="shared" si="9"/>
+      <c r="L154" s="65">
+        <f t="shared" si="17"/>
         <v>5.5519345135681117E-2</v>
       </c>
     </row>
-    <row r="140" spans="3:12" ht="28.9" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="C140" s="37" t="s">
+    <row r="155" spans="3:12" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C155" s="37" t="s">
         <v>29</v>
       </c>
-      <c r="D140" s="26">
+      <c r="D155" s="26">
         <v>19494</v>
       </c>
-      <c r="E140" s="28">
+      <c r="E155" s="28">
         <v>383792</v>
       </c>
-      <c r="F140" s="62">
+      <c r="F155" s="61">
         <v>221947</v>
       </c>
-      <c r="G140" s="60">
+      <c r="G155" s="59">
         <v>2399574</v>
       </c>
-      <c r="I140" s="67">
-        <f t="shared" ref="I140:I143" si="10">D140/SUM(D$139:D$143)</f>
+      <c r="I155" s="65">
+        <f t="shared" ref="I155:I158" si="18">D155/SUM(D$154:D$158)</f>
         <v>1.6797845077922906E-2</v>
       </c>
-      <c r="J140" s="67">
-        <f t="shared" si="9"/>
+      <c r="J155" s="65">
+        <f t="shared" si="17"/>
         <v>0.19546449760044249</v>
       </c>
-      <c r="K140" s="67">
-        <f t="shared" si="9"/>
+      <c r="K155" s="65">
+        <f t="shared" si="17"/>
         <v>2.7820336483339096E-2</v>
       </c>
-      <c r="L140" s="67">
-        <f t="shared" si="9"/>
+      <c r="L155" s="65">
+        <f t="shared" si="17"/>
         <v>0.18681467714716976</v>
       </c>
     </row>
-    <row r="141" spans="3:12" ht="28.9" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="C141" s="37" t="s">
+    <row r="156" spans="3:12" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C156" s="37" t="s">
         <v>30</v>
       </c>
-      <c r="D141" s="26">
+      <c r="D156" s="26">
         <v>208032</v>
       </c>
-      <c r="E141" s="28">
+      <c r="E156" s="28">
         <v>576634</v>
       </c>
-      <c r="F141" s="62">
+      <c r="F156" s="61">
         <v>1998546</v>
       </c>
-      <c r="G141" s="60">
+      <c r="G156" s="59">
         <v>2418598</v>
       </c>
-      <c r="I141" s="67">
-        <f t="shared" si="10"/>
+      <c r="I156" s="65">
+        <f t="shared" si="18"/>
         <v>0.17925973670105971</v>
       </c>
-      <c r="J141" s="67">
-        <f t="shared" si="9"/>
+      <c r="J156" s="65">
+        <f t="shared" si="17"/>
         <v>0.2936785423076394</v>
       </c>
-      <c r="K141" s="67">
-        <f t="shared" si="9"/>
+      <c r="K156" s="65">
+        <f t="shared" si="17"/>
         <v>0.25051125808157543</v>
       </c>
-      <c r="L141" s="67">
-        <f t="shared" si="9"/>
+      <c r="L156" s="65">
+        <f t="shared" si="17"/>
         <v>0.18829575771315679</v>
       </c>
     </row>
-    <row r="142" spans="3:12" ht="28.9" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="C142" s="37" t="s">
+    <row r="157" spans="3:12" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C157" s="37" t="s">
         <v>31</v>
       </c>
-      <c r="D142" s="26">
+      <c r="D157" s="26">
         <v>758924</v>
       </c>
-      <c r="E142" s="28">
+      <c r="E157" s="28">
         <v>296755</v>
       </c>
-      <c r="F142" s="62">
+      <c r="F157" s="61">
         <v>4665672</v>
       </c>
-      <c r="G142" s="60">
+      <c r="G157" s="59">
         <v>1745044</v>
       </c>
-      <c r="I142" s="67">
-        <f t="shared" si="10"/>
+      <c r="I157" s="65">
+        <f t="shared" si="18"/>
         <v>0.65395956591348947</v>
       </c>
-      <c r="J142" s="67">
-        <f t="shared" si="9"/>
+      <c r="J157" s="65">
+        <f t="shared" si="17"/>
         <v>0.15113672766868333</v>
       </c>
-      <c r="K142" s="67">
-        <f t="shared" si="9"/>
+      <c r="K157" s="65">
+        <f t="shared" si="17"/>
         <v>0.58482685037821502</v>
       </c>
-      <c r="L142" s="67">
-        <f t="shared" si="9"/>
+      <c r="L157" s="65">
+        <f t="shared" si="17"/>
         <v>0.13585737779606119</v>
       </c>
     </row>
-    <row r="143" spans="3:12" ht="28.9" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="C143" s="37" t="s">
+    <row r="158" spans="3:12" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C158" s="37" t="s">
         <v>32</v>
       </c>
-      <c r="D143" s="26">
+      <c r="D158" s="26">
         <v>172875</v>
       </c>
-      <c r="E143" s="28">
+      <c r="E158" s="28">
         <v>578515</v>
       </c>
-      <c r="F143" s="62">
+      <c r="F158" s="61">
         <v>1089298</v>
       </c>
-      <c r="G143" s="60">
+      <c r="G158" s="59">
         <v>5568332</v>
       </c>
-      <c r="I143" s="67">
-        <f t="shared" si="10"/>
+      <c r="I158" s="65">
+        <f t="shared" si="18"/>
         <v>0.14896519276936096</v>
       </c>
-      <c r="J143" s="67">
-        <f t="shared" si="9"/>
+      <c r="J158" s="65">
+        <f t="shared" si="17"/>
         <v>0.29463653184360272</v>
       </c>
-      <c r="K143" s="67">
-        <f t="shared" si="9"/>
+      <c r="K158" s="65">
+        <f t="shared" si="17"/>
         <v>0.13653997076161567</v>
       </c>
-      <c r="L143" s="67">
-        <f t="shared" si="9"/>
+      <c r="L158" s="65">
+        <f t="shared" si="17"/>
         <v>0.43351284220793113</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="4">
-    <mergeCell ref="D136:E136"/>
-    <mergeCell ref="F136:G136"/>
-    <mergeCell ref="C106:C107"/>
-    <mergeCell ref="C104:C105"/>
+    <mergeCell ref="D151:E151"/>
+    <mergeCell ref="F151:G151"/>
+    <mergeCell ref="C121:C122"/>
+    <mergeCell ref="C119:C120"/>
   </mergeCells>
-  <conditionalFormatting sqref="B42:G42 B74:H77">
-    <cfRule type="expression" dxfId="10" priority="16">
-      <formula>ISERROR($F42)</formula>
+  <conditionalFormatting sqref="B57:G57 B89:H92">
+    <cfRule type="expression" dxfId="10" priority="17">
+      <formula>ISERROR($F57)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B43:G43">
-    <cfRule type="expression" dxfId="9" priority="15">
-      <formula>ISERROR($F43)</formula>
+  <conditionalFormatting sqref="B58:G58">
+    <cfRule type="expression" dxfId="9" priority="16">
+      <formula>ISERROR($F58)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B44:G44">
-    <cfRule type="expression" dxfId="8" priority="14">
-      <formula>ISERROR($F44)</formula>
+  <conditionalFormatting sqref="B59:G59">
+    <cfRule type="expression" dxfId="8" priority="15">
+      <formula>ISERROR($F59)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="O74:S74">
-    <cfRule type="expression" dxfId="7" priority="11">
-      <formula>ISERROR($F74)</formula>
+  <conditionalFormatting sqref="O89:S89">
+    <cfRule type="expression" dxfId="7" priority="12">
+      <formula>ISERROR($F89)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="O75:S75">
-    <cfRule type="expression" dxfId="6" priority="10">
-      <formula>ISERROR($F75)</formula>
+  <conditionalFormatting sqref="O90:S90">
+    <cfRule type="expression" dxfId="6" priority="11">
+      <formula>ISERROR($F90)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="O76:S76">
-    <cfRule type="expression" dxfId="5" priority="9">
-      <formula>ISERROR($F76)</formula>
+  <conditionalFormatting sqref="O91:S91">
+    <cfRule type="expression" dxfId="5" priority="10">
+      <formula>ISERROR($F91)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="O77:S77">
-    <cfRule type="expression" dxfId="4" priority="8">
-      <formula>ISERROR($F77)</formula>
+  <conditionalFormatting sqref="O92:S92">
+    <cfRule type="expression" dxfId="4" priority="9">
+      <formula>ISERROR($F92)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E106:I107">
-    <cfRule type="expression" dxfId="3" priority="17">
-      <formula>ISERROR($H106)</formula>
+  <conditionalFormatting sqref="E121:I122">
+    <cfRule type="expression" dxfId="3" priority="18">
+      <formula>ISERROR($H121)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D106:D107">
-    <cfRule type="expression" dxfId="2" priority="4">
-      <formula>ISERROR($H106)</formula>
+  <conditionalFormatting sqref="D121:D122">
+    <cfRule type="expression" dxfId="2" priority="5">
+      <formula>ISERROR($H121)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C139:D143">
-    <cfRule type="expression" dxfId="1" priority="19">
+  <conditionalFormatting sqref="C154:D158">
+    <cfRule type="expression" dxfId="1" priority="20">
       <formula>ISERROR(#REF!)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B38:D42 G38:I42">
+    <cfRule type="expression" dxfId="0" priority="22">
+      <formula>ISERROR($G38)</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
subset data to female only for regressions
</commit_message>
<xml_diff>
--- a/OUTPUT/DATA/Charting.xlsx
+++ b/OUTPUT/DATA/Charting.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="M:\Work\Childcare and parental employment\childcare\OUTPUT\DATA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E065364-C4C8-4BDC-AEF7-9E917FED4458}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C1877B7-27F8-4829-B4B6-DFB49F85DB67}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-3735" yWindow="8002" windowWidth="20715" windowHeight="13276" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="39">
   <si>
     <t>Barchart showing employment rates, parents vs. non-parents, by overall, sex and region</t>
   </si>
@@ -136,6 +136,21 @@
   </si>
   <si>
     <t>Composition of parents in London vs. UK by age group, 2022</t>
+  </si>
+  <si>
+    <t>London female parents vs. UK female parents</t>
+  </si>
+  <si>
+    <t>lmin</t>
+  </si>
+  <si>
+    <t>lmax</t>
+  </si>
+  <si>
+    <t>umin</t>
+  </si>
+  <si>
+    <t>umax</t>
   </si>
 </sst>
 </file>
@@ -1539,7 +1554,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$C$53</c:f>
+              <c:f>Sheet1!$C$59</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1564,7 +1579,7 @@
             <c:noEndCap val="0"/>
             <c:plus>
               <c:numRef>
-                <c:f>Sheet1!$D$55:$D$59</c:f>
+                <c:f>Sheet1!$D$61:$D$65</c:f>
                 <c:numCache>
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="5"/>
@@ -1588,7 +1603,7 @@
             </c:plus>
             <c:minus>
               <c:numRef>
-                <c:f>Sheet1!$D$55:$D$59</c:f>
+                <c:f>Sheet1!$D$61:$D$65</c:f>
                 <c:numCache>
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="5"/>
@@ -1626,7 +1641,7 @@
           </c:errBars>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$B$55:$B$59</c:f>
+              <c:f>Sheet1!$B$61:$B$65</c:f>
               <c:strCache>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
@@ -1649,7 +1664,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$C$55:$C$59</c:f>
+              <c:f>Sheet1!$C$61:$C$65</c:f>
               <c:numCache>
                 <c:formatCode>0.0%</c:formatCode>
                 <c:ptCount val="5"/>
@@ -1682,7 +1697,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$F$53</c:f>
+              <c:f>Sheet1!$F$59</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1707,7 +1722,7 @@
             <c:noEndCap val="0"/>
             <c:plus>
               <c:numRef>
-                <c:f>Sheet1!$G$55:$G$59</c:f>
+                <c:f>Sheet1!$G$61:$G$65</c:f>
                 <c:numCache>
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="5"/>
@@ -1731,7 +1746,7 @@
             </c:plus>
             <c:minus>
               <c:numRef>
-                <c:f>Sheet1!$G$55:$G$59</c:f>
+                <c:f>Sheet1!$G$61:$G$65</c:f>
                 <c:numCache>
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="5"/>
@@ -1769,7 +1784,7 @@
           </c:errBars>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$B$55:$B$59</c:f>
+              <c:f>Sheet1!$B$61:$B$65</c:f>
               <c:strCache>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
@@ -1792,7 +1807,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$F$55:$F$59</c:f>
+              <c:f>Sheet1!$F$61:$F$65</c:f>
               <c:numCache>
                 <c:formatCode>0.0%</c:formatCode>
                 <c:ptCount val="5"/>
@@ -2119,7 +2134,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$C$53</c:f>
+              <c:f>Sheet1!$C$59</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -2140,7 +2155,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$B$88:$B$92</c:f>
+              <c:f>Sheet1!$B$94:$B$98</c:f>
               <c:strCache>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
@@ -2163,7 +2178,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$K$88:$K$92</c:f>
+              <c:f>Sheet1!$K$94:$K$98</c:f>
               <c:numCache>
                 <c:formatCode>0%</c:formatCode>
                 <c:ptCount val="5"/>
@@ -2196,7 +2211,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$F$53</c:f>
+              <c:f>Sheet1!$F$59</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -2217,7 +2232,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$B$88:$B$92</c:f>
+              <c:f>Sheet1!$B$94:$B$98</c:f>
               <c:strCache>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
@@ -2240,7 +2255,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$L$88:$L$92</c:f>
+              <c:f>Sheet1!$L$94:$L$98</c:f>
               <c:numCache>
                 <c:formatCode>0%</c:formatCode>
                 <c:ptCount val="5"/>
@@ -2565,7 +2580,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$C$53</c:f>
+              <c:f>Sheet1!$C$59</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -2586,7 +2601,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$B$88:$B$92</c:f>
+              <c:f>Sheet1!$B$94:$B$98</c:f>
               <c:strCache>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
@@ -2609,7 +2624,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$Q$88:$Q$92</c:f>
+              <c:f>Sheet1!$Q$94:$Q$98</c:f>
               <c:numCache>
                 <c:formatCode>#,##0</c:formatCode>
                 <c:ptCount val="5"/>
@@ -2642,7 +2657,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$F$53</c:f>
+              <c:f>Sheet1!$F$59</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -2663,7 +2678,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$B$88:$B$92</c:f>
+              <c:f>Sheet1!$B$94:$B$98</c:f>
               <c:strCache>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
@@ -2686,7 +2701,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$T$88:$T$92</c:f>
+              <c:f>Sheet1!$T$94:$T$98</c:f>
               <c:numCache>
                 <c:formatCode>_-* #,##0_-;\-* #,##0_-;_-* "-"??_-;_-@_-</c:formatCode>
                 <c:ptCount val="5"/>
@@ -3011,7 +3026,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$E$117</c:f>
+              <c:f>Sheet1!$E$123</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -3036,7 +3051,7 @@
             <c:noEndCap val="0"/>
             <c:plus>
               <c:numRef>
-                <c:f>Sheet1!$F$119:$F$122</c:f>
+                <c:f>Sheet1!$F$125:$F$128</c:f>
                 <c:numCache>
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="4"/>
@@ -3057,7 +3072,7 @@
             </c:plus>
             <c:minus>
               <c:numRef>
-                <c:f>Sheet1!$F$119:$F$122</c:f>
+                <c:f>Sheet1!$F$125:$F$128</c:f>
                 <c:numCache>
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="4"/>
@@ -3092,7 +3107,7 @@
           </c:errBars>
           <c:cat>
             <c:multiLvlStrRef>
-              <c:f>Sheet1!$C$119:$D$122</c:f>
+              <c:f>Sheet1!$C$125:$D$128</c:f>
               <c:multiLvlStrCache>
                 <c:ptCount val="4"/>
                 <c:lvl>
@@ -3122,7 +3137,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$E$119:$E$122</c:f>
+              <c:f>Sheet1!$E$125:$E$128</c:f>
               <c:numCache>
                 <c:formatCode>0.0%</c:formatCode>
                 <c:ptCount val="4"/>
@@ -3152,7 +3167,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$H$117</c:f>
+              <c:f>Sheet1!$H$123</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -3177,7 +3192,7 @@
             <c:noEndCap val="0"/>
             <c:plus>
               <c:numRef>
-                <c:f>Sheet1!$I$119:$I$122</c:f>
+                <c:f>Sheet1!$I$125:$I$128</c:f>
                 <c:numCache>
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="4"/>
@@ -3198,7 +3213,7 @@
             </c:plus>
             <c:minus>
               <c:numRef>
-                <c:f>Sheet1!$I$119:$I$122</c:f>
+                <c:f>Sheet1!$I$125:$I$128</c:f>
                 <c:numCache>
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="4"/>
@@ -3233,7 +3248,7 @@
           </c:errBars>
           <c:cat>
             <c:multiLvlStrRef>
-              <c:f>Sheet1!$C$119:$D$122</c:f>
+              <c:f>Sheet1!$C$125:$D$128</c:f>
               <c:multiLvlStrCache>
                 <c:ptCount val="4"/>
                 <c:lvl>
@@ -3263,7 +3278,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$H$119:$H$122</c:f>
+              <c:f>Sheet1!$H$125:$H$128</c:f>
               <c:numCache>
                 <c:formatCode>0.0%</c:formatCode>
                 <c:ptCount val="4"/>
@@ -3595,7 +3610,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$C$154</c:f>
+              <c:f>Sheet1!$C$160</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -3760,7 +3775,7 @@
           </c:dLbls>
           <c:cat>
             <c:multiLvlStrRef>
-              <c:f>Sheet1!$D$151:$G$152</c:f>
+              <c:f>Sheet1!$D$157:$G$158</c:f>
               <c:multiLvlStrCache>
                 <c:ptCount val="4"/>
                 <c:lvl>
@@ -3790,7 +3805,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$D$154:$G$154</c:f>
+              <c:f>Sheet1!$D$160:$G$160</c:f>
               <c:numCache>
                 <c:formatCode>_-* #,##0_-;\-* #,##0_-;_-* "-"??_-;_-@_-</c:formatCode>
                 <c:ptCount val="4"/>
@@ -3812,7 +3827,7 @@
           <c:extLst>
             <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
               <c15:datalabelsRange>
-                <c15:f>Sheet1!$I$154:$L$154</c15:f>
+                <c15:f>Sheet1!$I$160:$L$160</c15:f>
                 <c15:dlblRangeCache>
                   <c:ptCount val="4"/>
                   <c:pt idx="0">
@@ -3840,7 +3855,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$C$155</c:f>
+              <c:f>Sheet1!$C$161</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -4044,7 +4059,7 @@
           </c:dLbls>
           <c:cat>
             <c:multiLvlStrRef>
-              <c:f>Sheet1!$D$151:$G$152</c:f>
+              <c:f>Sheet1!$D$157:$G$158</c:f>
               <c:multiLvlStrCache>
                 <c:ptCount val="4"/>
                 <c:lvl>
@@ -4074,7 +4089,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$D$155:$G$155</c:f>
+              <c:f>Sheet1!$D$161:$G$161</c:f>
               <c:numCache>
                 <c:formatCode>_-* #,##0_-;\-* #,##0_-;_-* "-"??_-;_-@_-</c:formatCode>
                 <c:ptCount val="4"/>
@@ -4096,7 +4111,7 @@
           <c:extLst>
             <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
               <c15:datalabelsRange>
-                <c15:f>Sheet1!$I$155:$L$155</c15:f>
+                <c15:f>Sheet1!$I$161:$L$161</c15:f>
                 <c15:dlblRangeCache>
                   <c:ptCount val="4"/>
                   <c:pt idx="0">
@@ -4124,7 +4139,7 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$C$156</c:f>
+              <c:f>Sheet1!$C$162</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -4328,7 +4343,7 @@
           </c:dLbls>
           <c:cat>
             <c:multiLvlStrRef>
-              <c:f>Sheet1!$D$151:$G$152</c:f>
+              <c:f>Sheet1!$D$157:$G$158</c:f>
               <c:multiLvlStrCache>
                 <c:ptCount val="4"/>
                 <c:lvl>
@@ -4358,7 +4373,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$D$156:$G$156</c:f>
+              <c:f>Sheet1!$D$162:$G$162</c:f>
               <c:numCache>
                 <c:formatCode>_-* #,##0_-;\-* #,##0_-;_-* "-"??_-;_-@_-</c:formatCode>
                 <c:ptCount val="4"/>
@@ -4380,7 +4395,7 @@
           <c:extLst>
             <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
               <c15:datalabelsRange>
-                <c15:f>Sheet1!$I$156:$L$156</c15:f>
+                <c15:f>Sheet1!$I$162:$L$162</c15:f>
                 <c15:dlblRangeCache>
                   <c:ptCount val="4"/>
                   <c:pt idx="0">
@@ -4408,7 +4423,7 @@
           <c:order val="3"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$C$157</c:f>
+              <c:f>Sheet1!$C$163</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -4612,7 +4627,7 @@
           </c:dLbls>
           <c:cat>
             <c:multiLvlStrRef>
-              <c:f>Sheet1!$D$151:$G$152</c:f>
+              <c:f>Sheet1!$D$157:$G$158</c:f>
               <c:multiLvlStrCache>
                 <c:ptCount val="4"/>
                 <c:lvl>
@@ -4642,7 +4657,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$D$157:$G$157</c:f>
+              <c:f>Sheet1!$D$163:$G$163</c:f>
               <c:numCache>
                 <c:formatCode>_-* #,##0_-;\-* #,##0_-;_-* "-"??_-;_-@_-</c:formatCode>
                 <c:ptCount val="4"/>
@@ -4664,7 +4679,7 @@
           <c:extLst>
             <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
               <c15:datalabelsRange>
-                <c15:f>Sheet1!$I$157:$L$157</c15:f>
+                <c15:f>Sheet1!$I$163:$L$163</c15:f>
                 <c15:dlblRangeCache>
                   <c:ptCount val="4"/>
                   <c:pt idx="0">
@@ -4692,7 +4707,7 @@
           <c:order val="4"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$C$158</c:f>
+              <c:f>Sheet1!$C$164</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -4896,7 +4911,7 @@
           </c:dLbls>
           <c:cat>
             <c:multiLvlStrRef>
-              <c:f>Sheet1!$D$151:$G$152</c:f>
+              <c:f>Sheet1!$D$157:$G$158</c:f>
               <c:multiLvlStrCache>
                 <c:ptCount val="4"/>
                 <c:lvl>
@@ -4926,7 +4941,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$D$158:$G$158</c:f>
+              <c:f>Sheet1!$D$164:$G$164</c:f>
               <c:numCache>
                 <c:formatCode>_-* #,##0_-;\-* #,##0_-;_-* "-"??_-;_-@_-</c:formatCode>
                 <c:ptCount val="4"/>
@@ -4948,7 +4963,7 @@
           <c:extLst>
             <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
               <c15:datalabelsRange>
-                <c15:f>Sheet1!$I$158:$L$158</c15:f>
+                <c15:f>Sheet1!$I$164:$L$164</c15:f>
                 <c15:dlblRangeCache>
                   <c:ptCount val="4"/>
                   <c:pt idx="0">
@@ -5168,6 +5183,691 @@
     <a:p>
       <a:pPr>
         <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart7.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-GB" b="1"/>
+              <a:t>Employment rate,</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-GB" b="1" baseline="0"/>
+              <a:t> female parents</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-GB" b="1"/>
+              <a:t>, 2018-2022</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="1.9416666666666652E-2"/>
+          <c:y val="2.2727272727272728E-2"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:areaChart>
+        <c:grouping val="stacked"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$N$37</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>lmin</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln w="25400">
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$N$38:$N$42</c:f>
+              <c:numCache>
+                <c:formatCode>0.0%</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>0.67070957270610998</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.67534028762930876</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.67890648670510312</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.68601687503403153</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.67575157693449572</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-20C4-44A8-A5CA-0165BF5104E9}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$O$37</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>lmax</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1">
+                <a:lumMod val="20000"/>
+                <a:lumOff val="80000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:ln w="25400">
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$O$38:$O$42</c:f>
+              <c:numCache>
+                <c:formatCode>0.0%</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>2.6060549218728024E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.6856977483998401E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3.2339718410387741E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3.271041115092288E-2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>3.4637029809506448E-2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-20C4-44A8-A5CA-0165BF5104E9}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="5"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$P$37</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>umin</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln w="25400">
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$P$38:$P$42</c:f>
+              <c:numCache>
+                <c:formatCode>0.0%</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>4.1048370867461048E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4.4288656140220817E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3.782899966567399E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3.2086818103311487E-2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>3.9829259390829819E-2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-20C4-44A8-A5CA-0165BF5104E9}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="5"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$Q$37</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>umax</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2">
+                <a:lumMod val="20000"/>
+                <a:lumOff val="80000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:ln w="25400">
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$Q$38:$Q$42</c:f>
+              <c:numCache>
+                <c:formatCode>0.0%</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>8.3920848192557962E-3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>8.5144671961021601E-3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.021825034791024E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.056007149377014E-2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.0894423690529953E-2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-20C4-44A8-A5CA-0165BF5104E9}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="313329504"/>
+        <c:axId val="313330160"/>
+      </c:areaChart>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$C$36</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>London</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$B$8:$B$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>2018</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2019</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2020</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2021</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2022</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$C$38:$C$42</c:f>
+              <c:numCache>
+                <c:formatCode>0.0%</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>0.68373984731547399</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.68876877637130796</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.69507634591029699</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.70237208060949297</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.69307009183924895</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000004-20C4-44A8-A5CA-0165BF5104E9}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$H$36</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>UK</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$H$38:$H$42</c:f>
+              <c:numCache>
+                <c:formatCode>0.0%</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>0.74201453520192695</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.75074315485157905</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.75418432995511997</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.75609414003515096</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.75566507798009697</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000005-20C4-44A8-A5CA-0165BF5104E9}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="313329504"/>
+        <c:axId val="313330160"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="313329504"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="313330160"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="313330160"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="0%" sourceLinked="0"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="313329504"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+        <c:majorUnit val="5.000000000000001E-2"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="t"/>
+      <c:legendEntry>
+        <c:idx val="0"/>
+        <c:delete val="1"/>
+      </c:legendEntry>
+      <c:legendEntry>
+        <c:idx val="1"/>
+        <c:delete val="1"/>
+      </c:legendEntry>
+      <c:legendEntry>
+        <c:idx val="2"/>
+        <c:delete val="1"/>
+      </c:legendEntry>
+      <c:legendEntry>
+        <c:idx val="3"/>
+        <c:delete val="1"/>
+      </c:legendEntry>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="3.2996281714785636E-2"/>
+          <c:y val="0.14136363636363636"/>
+          <c:w val="0.27800850368834246"/>
+          <c:h val="6.2257248244319108E-2"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:noFill/>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr>
+          <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+          <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+        </a:defRPr>
       </a:pPr>
       <a:endParaRPr lang="en-US"/>
     </a:p>
@@ -5420,6 +6120,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors7.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
   <cs:axisTitle>
@@ -8098,6 +8838,522 @@
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style7.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
       <a:ln w="9525">
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -8493,13 +9749,13 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>106361</xdr:colOff>
-      <xdr:row>60</xdr:row>
+      <xdr:row>66</xdr:row>
       <xdr:rowOff>144461</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
       <xdr:colOff>96837</xdr:colOff>
-      <xdr:row>81</xdr:row>
+      <xdr:row>87</xdr:row>
       <xdr:rowOff>106361</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -8529,13 +9785,13 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>93</xdr:row>
+      <xdr:row>99</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
       <xdr:colOff>635001</xdr:colOff>
-      <xdr:row>113</xdr:row>
+      <xdr:row>119</xdr:row>
       <xdr:rowOff>146050</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -8567,13 +9823,13 @@
     <xdr:from>
       <xdr:col>12</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>93</xdr:row>
+      <xdr:row>99</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>21</xdr:col>
       <xdr:colOff>90488</xdr:colOff>
-      <xdr:row>113</xdr:row>
+      <xdr:row>119</xdr:row>
       <xdr:rowOff>144462</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -8605,13 +9861,13 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>641350</xdr:colOff>
-      <xdr:row>124</xdr:row>
+      <xdr:row>130</xdr:row>
       <xdr:rowOff>57150</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
       <xdr:colOff>630238</xdr:colOff>
-      <xdr:row>145</xdr:row>
+      <xdr:row>151</xdr:row>
       <xdr:rowOff>17462</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -8643,13 +9899,13 @@
     <xdr:from>
       <xdr:col>5</xdr:col>
       <xdr:colOff>25400</xdr:colOff>
-      <xdr:row>135</xdr:row>
+      <xdr:row>141</xdr:row>
       <xdr:rowOff>165100</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
       <xdr:colOff>469900</xdr:colOff>
-      <xdr:row>140</xdr:row>
+      <xdr:row>146</xdr:row>
       <xdr:rowOff>133350</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -8709,13 +9965,13 @@
     <xdr:from>
       <xdr:col>2</xdr:col>
       <xdr:colOff>247200</xdr:colOff>
-      <xdr:row>128</xdr:row>
+      <xdr:row>134</xdr:row>
       <xdr:rowOff>87152</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
       <xdr:colOff>247560</xdr:colOff>
-      <xdr:row>128</xdr:row>
+      <xdr:row>134</xdr:row>
       <xdr:rowOff>90687</xdr:rowOff>
     </xdr:to>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
@@ -8774,13 +10030,13 @@
     <xdr:from>
       <xdr:col>12</xdr:col>
       <xdr:colOff>634830</xdr:colOff>
-      <xdr:row>78</xdr:row>
+      <xdr:row>84</xdr:row>
       <xdr:rowOff>86160</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
       <xdr:colOff>607509</xdr:colOff>
-      <xdr:row>78</xdr:row>
+      <xdr:row>84</xdr:row>
       <xdr:rowOff>90268</xdr:rowOff>
     </xdr:to>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
@@ -8839,13 +10095,13 @@
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>160</xdr:row>
+      <xdr:row>166</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
       <xdr:colOff>638176</xdr:colOff>
-      <xdr:row>180</xdr:row>
+      <xdr:row>186</xdr:row>
       <xdr:rowOff>144462</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -8868,6 +10124,44 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId10"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>352425</xdr:colOff>
+      <xdr:row>42</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>797719</xdr:colOff>
+      <xdr:row>59</xdr:row>
+      <xdr:rowOff>177006</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="11" name="Chart 10">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{87574711-08DA-4ED8-802F-1C972E07578F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId11"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -9231,10 +10525,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B3:T158"/>
+  <dimension ref="B3:T164"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
-      <selection activeCell="N32" sqref="N32"/>
+    <sheetView tabSelected="1" topLeftCell="A33" workbookViewId="0">
+      <selection activeCell="P50" sqref="P50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9591,16 +10885,21 @@
         <v>2.2535686420780854E-2</v>
       </c>
     </row>
+    <row r="34" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="C34" t="s">
+        <v>34</v>
+      </c>
+    </row>
     <row r="35" spans="2:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="36" spans="2:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C36" s="1" t="s">
-        <v>2</v>
+        <v>27</v>
       </c>
       <c r="D36" s="2"/>
       <c r="E36" s="3"/>
       <c r="G36" s="2"/>
       <c r="H36" s="1" t="s">
-        <v>3</v>
+        <v>26</v>
       </c>
     </row>
     <row r="37" spans="2:17" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -9636,16 +10935,16 @@
         <v>6</v>
       </c>
       <c r="N37" s="29" t="s">
-        <v>10</v>
+        <v>35</v>
       </c>
       <c r="O37" s="29" t="s">
-        <v>11</v>
+        <v>36</v>
       </c>
       <c r="P37" s="29" t="s">
-        <v>9</v>
+        <v>37</v>
       </c>
       <c r="Q37" s="29" t="s">
-        <v>12</v>
+        <v>38</v>
       </c>
     </row>
     <row r="38" spans="2:17" x14ac:dyDescent="0.25">
@@ -9670,37 +10969,37 @@
         <v>1147726</v>
       </c>
       <c r="H38" s="12">
-        <v>0.68203239181976605</v>
+        <v>0.74201453520192695</v>
       </c>
       <c r="I38" s="15">
-        <v>1.11446599426694E-2</v>
+        <v>4.1960424096278998E-3</v>
       </c>
       <c r="J38" s="15">
         <f>H38+I38</f>
-        <v>0.69317705176243549</v>
+        <v>0.74621057761155485</v>
       </c>
       <c r="K38" s="15">
         <f>H38-I38</f>
-        <v>0.6708877318770966</v>
+        <v>0.73781849279229905</v>
       </c>
       <c r="L38" s="16">
-        <v>1847380</v>
+        <v>7829131</v>
       </c>
       <c r="N38" s="30">
-        <f>K38</f>
-        <v>0.6708877318770966</v>
+        <f>F38</f>
+        <v>0.67070957270610998</v>
       </c>
       <c r="O38" s="30">
-        <f>J38-K38</f>
-        <v>2.2289319885338887E-2</v>
-      </c>
-      <c r="P38" s="30">
-        <f>F38-J38</f>
-        <v>-2.2467479056325512E-2</v>
-      </c>
-      <c r="Q38" s="30">
         <f>E38-F38</f>
         <v>2.6060549218728024E-2</v>
+      </c>
+      <c r="P38" s="30">
+        <f>K38-E38</f>
+        <v>4.1048370867461048E-2</v>
+      </c>
+      <c r="Q38" s="30">
+        <f>J38-K38</f>
+        <v>8.3920848192557962E-3</v>
       </c>
     </row>
     <row r="39" spans="2:17" x14ac:dyDescent="0.25">
@@ -9725,37 +11024,37 @@
         <v>1185000</v>
       </c>
       <c r="H39" s="18">
-        <v>0.68767282696699705</v>
+        <v>0.75074315485157905</v>
       </c>
       <c r="I39" s="19">
-        <v>1.13776465862128E-2</v>
+        <v>4.2572335980511199E-3</v>
       </c>
       <c r="J39" s="19">
         <f t="shared" ref="J39:J42" si="10">H39+I39</f>
-        <v>0.69905047355320982</v>
+        <v>0.75500038844963013</v>
       </c>
       <c r="K39" s="19">
         <f t="shared" ref="K39:K42" si="11">H39-I39</f>
-        <v>0.67629518038078429</v>
+        <v>0.74648592125352797</v>
       </c>
       <c r="L39" s="22">
-        <v>1861327</v>
+        <v>7865790</v>
       </c>
       <c r="N39" s="30">
-        <f t="shared" ref="N39:N42" si="12">K39</f>
-        <v>0.67629518038078429</v>
+        <f t="shared" ref="N39:N42" si="12">F39</f>
+        <v>0.67534028762930876</v>
       </c>
       <c r="O39" s="30">
-        <f t="shared" ref="O39:O42" si="13">J39-K39</f>
-        <v>2.2755293172425528E-2</v>
+        <f t="shared" ref="O39:O42" si="13">E39-F39</f>
+        <v>2.6856977483998401E-2</v>
       </c>
       <c r="P39" s="30">
-        <f t="shared" ref="P39:P42" si="14">F39-J39</f>
-        <v>-2.3710185923901061E-2</v>
+        <f t="shared" ref="P39:P42" si="14">K39-E39</f>
+        <v>4.4288656140220817E-2</v>
       </c>
       <c r="Q39" s="30">
-        <f t="shared" ref="Q39:Q42" si="15">E39-F39</f>
-        <v>2.6856977483998401E-2</v>
+        <f t="shared" ref="Q39:Q42" si="15">J39-K39</f>
+        <v>8.5144671961021601E-3</v>
       </c>
     </row>
     <row r="40" spans="2:17" x14ac:dyDescent="0.25">
@@ -9780,37 +11079,37 @@
         <v>1171772</v>
       </c>
       <c r="H40" s="18">
-        <v>0.70641098894904497</v>
+        <v>0.75418432995511997</v>
       </c>
       <c r="I40" s="19">
-        <v>1.4645902095903499E-2</v>
+        <v>5.1091251739551402E-3</v>
       </c>
       <c r="J40" s="19">
         <f t="shared" si="10"/>
-        <v>0.72105689104494852</v>
+        <v>0.75929345512907509</v>
       </c>
       <c r="K40" s="19">
         <f t="shared" si="11"/>
-        <v>0.69176508685314142</v>
+        <v>0.74907520478116485</v>
       </c>
       <c r="L40" s="22">
-        <v>1951415</v>
+        <v>7870137</v>
       </c>
       <c r="N40" s="30">
         <f t="shared" si="12"/>
-        <v>0.69176508685314142</v>
+        <v>0.67890648670510312</v>
       </c>
       <c r="O40" s="30">
         <f t="shared" si="13"/>
-        <v>2.9291804191807103E-2</v>
+        <v>3.2339718410387741E-2</v>
       </c>
       <c r="P40" s="30">
         <f t="shared" si="14"/>
-        <v>-4.2150404339845404E-2</v>
+        <v>3.782899966567399E-2</v>
       </c>
       <c r="Q40" s="30">
         <f t="shared" si="15"/>
-        <v>3.2339718410387741E-2</v>
+        <v>1.021825034791024E-2</v>
       </c>
     </row>
     <row r="41" spans="2:17" x14ac:dyDescent="0.25">
@@ -9835,37 +11134,37 @@
         <v>1154008</v>
       </c>
       <c r="H41" s="18">
-        <v>0.70862683351288602</v>
+        <v>0.75609414003515096</v>
       </c>
       <c r="I41" s="19">
-        <v>1.21421072255011E-2</v>
+        <v>5.28003574688509E-3</v>
       </c>
       <c r="J41" s="19">
         <f t="shared" si="10"/>
-        <v>0.72076894073838715</v>
+        <v>0.76137417578203603</v>
       </c>
       <c r="K41" s="19">
         <f t="shared" si="11"/>
-        <v>0.69648472628738489</v>
+        <v>0.75081410428826589</v>
       </c>
       <c r="L41" s="22">
-        <v>1930720</v>
+        <v>7949604</v>
       </c>
       <c r="N41" s="30">
         <f t="shared" si="12"/>
-        <v>0.69648472628738489</v>
+        <v>0.68601687503403153</v>
       </c>
       <c r="O41" s="30">
         <f t="shared" si="13"/>
-        <v>2.4284214451002262E-2</v>
+        <v>3.271041115092288E-2</v>
       </c>
       <c r="P41" s="30">
         <f t="shared" si="14"/>
-        <v>-3.4752065704355628E-2</v>
+        <v>3.2086818103311487E-2</v>
       </c>
       <c r="Q41" s="30">
         <f t="shared" si="15"/>
-        <v>3.271041115092288E-2</v>
+        <v>1.056007149377014E-2</v>
       </c>
     </row>
     <row r="42" spans="2:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -9890,927 +11189,927 @@
         <v>1160506</v>
       </c>
       <c r="H42" s="32">
-        <v>0.69684902421049899</v>
+        <v>0.75566507798009697</v>
       </c>
       <c r="I42" s="33">
-        <v>1.4223407773721899E-2</v>
+        <v>5.4472118452649296E-3</v>
       </c>
       <c r="J42" s="25">
         <f t="shared" si="10"/>
-        <v>0.71107243198422088</v>
+        <v>0.76111228982536194</v>
       </c>
       <c r="K42" s="25">
         <f t="shared" si="11"/>
-        <v>0.68262561643677711</v>
+        <v>0.75021786613483199</v>
       </c>
       <c r="L42" s="35">
-        <v>1963487</v>
+        <v>7977869</v>
       </c>
       <c r="N42" s="30">
         <f t="shared" si="12"/>
-        <v>0.68262561643677711</v>
+        <v>0.67575157693449572</v>
       </c>
       <c r="O42" s="30">
         <f t="shared" si="13"/>
-        <v>2.8446815547443771E-2</v>
+        <v>3.4637029809506448E-2</v>
       </c>
       <c r="P42" s="30">
         <f t="shared" si="14"/>
-        <v>-3.5320855049725153E-2</v>
+        <v>3.9829259390829819E-2</v>
       </c>
       <c r="Q42" s="30">
         <f t="shared" si="15"/>
-        <v>3.4637029809506448E-2</v>
+        <v>1.0894423690529953E-2</v>
       </c>
     </row>
-    <row r="50" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B50" t="s">
+    <row r="56" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B56" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="53" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C53" s="1" t="s">
+    <row r="58" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="59" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C59" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D53" s="2"/>
-      <c r="E53" s="3"/>
-      <c r="F53" s="1" t="s">
+      <c r="D59" s="2"/>
+      <c r="E59" s="3"/>
+      <c r="F59" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="G53" s="2"/>
-      <c r="H53" s="3"/>
+      <c r="G59" s="2"/>
+      <c r="H59" s="3"/>
     </row>
-    <row r="54" spans="2:8" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B54" s="4"/>
-      <c r="C54" s="5" t="s">
+    <row r="60" spans="2:8" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B60" s="4"/>
+      <c r="C60" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="D54" s="6" t="s">
+      <c r="D60" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="E54" s="7" t="s">
+      <c r="E60" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="F54" s="8" t="s">
+      <c r="F60" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="G54" s="9" t="s">
+      <c r="G60" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="H54" s="10" t="s">
+      <c r="H60" s="10" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="55" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B55" s="23" t="s">
+    <row r="61" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B61" s="23" t="s">
         <v>14</v>
       </c>
-      <c r="C55" s="24">
+      <c r="C61" s="24">
         <v>0.79933259145512303</v>
       </c>
-      <c r="D55" s="25">
+      <c r="D61" s="25">
         <v>1.1267843210390399E-2</v>
       </c>
-      <c r="E55" s="26">
+      <c r="E61" s="26">
         <v>2128831</v>
       </c>
-      <c r="F55" s="27">
+      <c r="F61" s="27">
         <v>0.712854868118178</v>
       </c>
-      <c r="G55" s="25">
+      <c r="G61" s="25">
         <v>1.03687839954644E-2</v>
       </c>
-      <c r="H55" s="28">
+      <c r="H61" s="28">
         <v>4121038</v>
       </c>
     </row>
-    <row r="56" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B56" s="23" t="s">
+    <row r="62" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B62" s="23" t="s">
         <v>15</v>
       </c>
-      <c r="C56" s="24">
+      <c r="C62" s="24">
         <v>0.92668473911135196</v>
       </c>
-      <c r="D56" s="25">
+      <c r="D62" s="25">
         <v>1.05909783386849E-2</v>
       </c>
-      <c r="E56" s="26">
+      <c r="E62" s="26">
         <v>968325</v>
       </c>
-      <c r="F56" s="27">
+      <c r="F62" s="27">
         <v>0.72742104358135695</v>
       </c>
-      <c r="G56" s="25">
+      <c r="G62" s="25">
         <v>1.3783532832492101E-2</v>
       </c>
-      <c r="H56" s="28">
+      <c r="H62" s="28">
         <v>2157551</v>
       </c>
     </row>
-    <row r="57" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B57" s="31" t="s">
+    <row r="63" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B63" s="31" t="s">
         <v>16</v>
       </c>
-      <c r="C57" s="32">
+      <c r="C63" s="32">
         <v>0.69307009183924895</v>
       </c>
-      <c r="D57" s="33">
+      <c r="D63" s="33">
         <v>1.73185149047532E-2</v>
       </c>
-      <c r="E57" s="34">
+      <c r="E63" s="34">
         <v>1160506</v>
       </c>
-      <c r="F57" s="32">
+      <c r="F63" s="32">
         <v>0.69684902421049899</v>
       </c>
-      <c r="G57" s="33">
+      <c r="G63" s="33">
         <v>1.4223407773721899E-2</v>
       </c>
-      <c r="H57" s="35">
+      <c r="H63" s="35">
         <v>1963487</v>
       </c>
     </row>
-    <row r="58" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B58" s="31" t="s">
+    <row r="64" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B64" s="31" t="s">
         <v>17</v>
       </c>
-      <c r="C58" s="32">
+      <c r="C64" s="32">
         <v>0.84620568430829102</v>
       </c>
-      <c r="D58" s="33">
+      <c r="D64" s="33">
         <v>1.36186819696885E-2</v>
       </c>
-      <c r="E58" s="34">
+      <c r="E64" s="34">
         <v>1102544</v>
       </c>
-      <c r="F58" s="32">
+      <c r="F64" s="32">
         <v>0.76244388299010402</v>
       </c>
-      <c r="G58" s="33">
+      <c r="G64" s="33">
         <v>1.2150622865273601E-2</v>
       </c>
-      <c r="H58" s="35">
+      <c r="H64" s="35">
         <v>2149972</v>
       </c>
     </row>
-    <row r="59" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B59" s="31" t="s">
+    <row r="65" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B65" s="31" t="s">
         <v>18</v>
       </c>
-      <c r="C59" s="32">
+      <c r="C65" s="32">
         <v>0.72710600508254997</v>
       </c>
-      <c r="D59" s="33">
+      <c r="D65" s="33">
         <v>1.8830962783656601E-2</v>
       </c>
-      <c r="E59" s="34">
+      <c r="E65" s="34">
         <v>899155</v>
       </c>
-      <c r="F59" s="32">
+      <c r="F65" s="32">
         <v>0.633415987774545</v>
       </c>
-      <c r="G59" s="33">
+      <c r="G65" s="33">
         <v>2.0722296241639598E-2</v>
       </c>
-      <c r="H59" s="35">
+      <c r="H65" s="35">
         <v>1296966</v>
       </c>
     </row>
-    <row r="84" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B84" t="s">
+    <row r="90" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B90" t="s">
         <v>19</v>
       </c>
-      <c r="O84" t="s">
+      <c r="O90" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="85" spans="2:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="86" spans="2:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D86" s="1" t="s">
+    <row r="91" spans="2:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="92" spans="2:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D92" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E86" s="2"/>
-      <c r="F86" s="3"/>
-      <c r="G86" s="1" t="s">
+      <c r="E92" s="2"/>
+      <c r="F92" s="3"/>
+      <c r="G92" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="H86" s="2"/>
-      <c r="I86" s="3"/>
-      <c r="O86" s="1" t="s">
+      <c r="H92" s="2"/>
+      <c r="I92" s="3"/>
+      <c r="O92" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="P86" s="2"/>
-      <c r="Q86" s="3"/>
-      <c r="R86" s="1" t="s">
+      <c r="P92" s="2"/>
+      <c r="Q92" s="3"/>
+      <c r="R92" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="S86" s="2"/>
-      <c r="T86" s="3"/>
+      <c r="S92" s="2"/>
+      <c r="T92" s="3"/>
     </row>
-    <row r="87" spans="2:20" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B87" s="36"/>
-      <c r="C87" s="4"/>
-      <c r="D87" s="5" t="s">
+    <row r="93" spans="2:20" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B93" s="36"/>
+      <c r="C93" s="4"/>
+      <c r="D93" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="E87" s="6" t="s">
+      <c r="E93" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="F87" s="7" t="s">
+      <c r="F93" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="G87" s="8" t="s">
+      <c r="G93" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="H87" s="9" t="s">
+      <c r="H93" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="I87" s="10" t="s">
+      <c r="I93" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="O87" s="5" t="s">
+      <c r="O93" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="P87" s="6" t="s">
+      <c r="P93" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="Q87" s="7" t="s">
+      <c r="Q93" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="R87" s="8" t="s">
+      <c r="R93" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="S87" s="9" t="s">
+      <c r="S93" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="T87" s="10" t="s">
+      <c r="T93" s="10" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="88" spans="2:20" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B88" s="37" t="s">
+    <row r="94" spans="2:20" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B94" s="37" t="s">
         <v>20</v>
       </c>
-      <c r="C88" s="23">
+      <c r="C94" s="23">
         <v>2022</v>
       </c>
-      <c r="D88" s="24">
+      <c r="D94" s="24">
         <v>0</v>
       </c>
-      <c r="E88" s="25">
+      <c r="E94" s="25">
         <v>0</v>
       </c>
-      <c r="F88" s="26">
+      <c r="F94" s="26">
         <v>2848</v>
       </c>
-      <c r="G88" s="27">
+      <c r="G94" s="27">
         <v>0.156390149230245</v>
       </c>
-      <c r="H88" s="25">
+      <c r="H94" s="25">
         <v>3.4288647309644198E-2</v>
       </c>
-      <c r="I88" s="28">
+      <c r="I94" s="28">
         <v>228774</v>
       </c>
-      <c r="K88" s="65">
-        <f>F88/SUM(F$88:F$92)</f>
+      <c r="K94" s="65">
+        <f>F94/SUM(F$94:F$98)</f>
         <v>1.337823434551639E-3</v>
       </c>
-      <c r="L88" s="65">
-        <f>G88/SUM(G$88:G$92)</f>
+      <c r="L94" s="65">
+        <f>G94/SUM(G$94:G$98)</f>
         <v>5.0123086443735511E-2</v>
       </c>
-      <c r="O88" s="24">
+      <c r="O94" s="24">
         <v>0</v>
       </c>
-      <c r="P88" s="25">
+      <c r="P94" s="25">
         <v>0</v>
       </c>
-      <c r="Q88" s="26">
+      <c r="Q94" s="26">
         <v>4073</v>
       </c>
-      <c r="R88" s="27">
+      <c r="R94" s="27">
         <v>0.22753347912538499</v>
       </c>
-      <c r="S88" s="25">
+      <c r="S94" s="25">
         <v>1.12995254747055E-2</v>
       </c>
-      <c r="T88" s="28">
+      <c r="T94" s="28">
         <v>1460985</v>
       </c>
     </row>
-    <row r="89" spans="2:20" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B89" s="37" t="s">
+    <row r="95" spans="2:20" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B95" s="37" t="s">
         <v>21</v>
       </c>
-      <c r="C89" s="31">
+      <c r="C95" s="31">
         <v>2022</v>
       </c>
-      <c r="D89" s="32">
+      <c r="D95" s="32">
         <v>0.37879936010777099</v>
       </c>
-      <c r="E89" s="33">
+      <c r="E95" s="33">
         <v>0.17094868918207601</v>
       </c>
-      <c r="F89" s="34">
+      <c r="F95" s="34">
         <v>23754</v>
       </c>
-      <c r="G89" s="32">
+      <c r="G95" s="32">
         <v>0.53690713703835602</v>
       </c>
-      <c r="H89" s="33">
+      <c r="H95" s="33">
         <v>2.5545960711472599E-2</v>
       </c>
-      <c r="I89" s="35">
+      <c r="I95" s="35">
         <v>820004</v>
       </c>
-      <c r="K89" s="65">
-        <f t="shared" ref="K89:L92" si="16">F89/SUM(F$88:F$92)</f>
+      <c r="K95" s="65">
+        <f t="shared" ref="K95:L98" si="16">F95/SUM(F$94:F$98)</f>
         <v>1.1158236609669815E-2</v>
       </c>
-      <c r="L89" s="65">
+      <c r="L95" s="65">
         <f t="shared" si="16"/>
         <v>0.17207888715811484</v>
       </c>
-      <c r="O89" s="32">
+      <c r="O95" s="32">
         <v>0.57470227417596398</v>
       </c>
-      <c r="P89" s="33">
+      <c r="P95" s="33">
         <v>5.5550415155696697E-2</v>
       </c>
-      <c r="Q89" s="34">
+      <c r="Q95" s="34">
         <v>287093</v>
       </c>
-      <c r="R89" s="32">
+      <c r="R95" s="32">
         <v>0.60569152688973105</v>
       </c>
-      <c r="S89" s="33">
+      <c r="S95" s="33">
         <v>1.18356916561004E-2</v>
       </c>
-      <c r="T89" s="35">
+      <c r="T95" s="35">
         <v>5068552</v>
       </c>
     </row>
-    <row r="90" spans="2:20" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B90" s="38" t="s">
+    <row r="96" spans="2:20" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B96" s="38" t="s">
         <v>22</v>
       </c>
-      <c r="C90" s="23">
+      <c r="C96" s="23">
         <v>2022</v>
       </c>
-      <c r="D90" s="24">
+      <c r="D96" s="24">
         <v>0.654116853960381</v>
       </c>
-      <c r="E90" s="25">
+      <c r="E96" s="25">
         <v>3.7122932812727799E-2</v>
       </c>
-      <c r="F90" s="26">
+      <c r="F96" s="26">
         <v>323378</v>
       </c>
-      <c r="G90" s="24">
+      <c r="G96" s="24">
         <v>0.86072573995033597</v>
       </c>
-      <c r="H90" s="25">
+      <c r="H96" s="25">
         <v>1.49910933603542E-2</v>
       </c>
-      <c r="I90" s="28">
+      <c r="I96" s="28">
         <v>1281809</v>
       </c>
-      <c r="K90" s="65">
+      <c r="K96" s="65">
         <f t="shared" si="16"/>
         <v>0.15190402620029492</v>
       </c>
-      <c r="L90" s="65">
+      <c r="L96" s="65">
         <f t="shared" si="16"/>
         <v>0.27586283970074654</v>
       </c>
-      <c r="O90" s="24">
+      <c r="O96" s="24">
         <v>0.77785784199696095</v>
       </c>
-      <c r="P90" s="25">
+      <c r="P96" s="25">
         <v>9.2520544076411804E-3</v>
       </c>
-      <c r="Q90" s="26">
+      <c r="Q96" s="26">
         <v>3125269</v>
       </c>
-      <c r="R90" s="24">
+      <c r="R96" s="24">
         <v>0.86854392893506704</v>
       </c>
-      <c r="S90" s="25">
+      <c r="S96" s="25">
         <v>5.9153296508353903E-3</v>
       </c>
-      <c r="T90" s="28">
+      <c r="T96" s="28">
         <v>5791661</v>
       </c>
     </row>
-    <row r="91" spans="2:20" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B91" s="37" t="s">
+    <row r="97" spans="2:20" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B97" s="37" t="s">
         <v>23</v>
       </c>
-      <c r="C91" s="23">
+      <c r="C97" s="23">
         <v>2022</v>
       </c>
-      <c r="D91" s="24">
+      <c r="D97" s="24">
         <v>0.83550437368352204</v>
       </c>
-      <c r="E91" s="25">
+      <c r="E97" s="25">
         <v>1.24987517244406E-2</v>
       </c>
-      <c r="F91" s="26">
+      <c r="F97" s="26">
         <v>1360638</v>
       </c>
-      <c r="G91" s="24">
+      <c r="G97" s="24">
         <v>0.88510018182858796</v>
       </c>
-      <c r="H91" s="25">
+      <c r="H97" s="25">
         <v>1.4664451939298301E-2</v>
       </c>
-      <c r="I91" s="28">
+      <c r="I97" s="28">
         <v>681411</v>
       </c>
-      <c r="K91" s="65">
+      <c r="K97" s="65">
         <f t="shared" si="16"/>
         <v>0.63914796430529242</v>
       </c>
-      <c r="L91" s="65">
+      <c r="L97" s="65">
         <f t="shared" si="16"/>
         <v>0.28367485512048218</v>
       </c>
-      <c r="O91" s="24">
+      <c r="O97" s="24">
         <v>0.858524078476263</v>
       </c>
-      <c r="P91" s="25">
+      <c r="P97" s="25">
         <v>4.2611303298503399E-3</v>
       </c>
-      <c r="Q91" s="26">
+      <c r="Q97" s="26">
         <v>8547094</v>
       </c>
-      <c r="R91" s="24">
+      <c r="R97" s="24">
         <v>0.85049191070230301</v>
       </c>
-      <c r="S91" s="25">
+      <c r="S97" s="25">
         <v>5.9803404560759997E-3</v>
       </c>
-      <c r="T91" s="28">
+      <c r="T97" s="28">
         <v>4132559</v>
       </c>
     </row>
-    <row r="92" spans="2:20" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B92" s="37" t="s">
+    <row r="98" spans="2:20" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B98" s="37" t="s">
         <v>24</v>
       </c>
-      <c r="C92" s="23">
+      <c r="C98" s="23">
         <v>2022</v>
       </c>
-      <c r="D92" s="24">
+      <c r="D98" s="24">
         <v>0.82326470004519203</v>
       </c>
-      <c r="E92" s="25">
+      <c r="E98" s="25">
         <v>2.22209055706417E-2</v>
       </c>
-      <c r="F92" s="26">
+      <c r="F98" s="26">
         <v>418213</v>
       </c>
-      <c r="G92" s="24">
+      <c r="G98" s="24">
         <v>0.68099888191589097</v>
       </c>
-      <c r="H92" s="25">
+      <c r="H98" s="25">
         <v>1.6739280203586698E-2</v>
       </c>
-      <c r="I92" s="28">
+      <c r="I98" s="28">
         <v>1109040</v>
       </c>
-      <c r="K92" s="65">
+      <c r="K98" s="65">
         <f t="shared" si="16"/>
         <v>0.1964519494501912</v>
       </c>
-      <c r="L92" s="65">
+      <c r="L98" s="65">
         <f t="shared" si="16"/>
         <v>0.21826033157692104</v>
       </c>
-      <c r="O92" s="24">
+      <c r="O98" s="24">
         <v>0.84478242876434095</v>
       </c>
-      <c r="P92" s="25">
+      <c r="P98" s="25">
         <v>7.8864302504463597E-3</v>
       </c>
-      <c r="Q92" s="26">
+      <c r="Q98" s="26">
         <v>2498538</v>
       </c>
-      <c r="R92" s="24">
+      <c r="R98" s="24">
         <v>0.68373064990839905</v>
       </c>
-      <c r="S92" s="25">
+      <c r="S98" s="25">
         <v>4.4157094066778497E-3</v>
       </c>
-      <c r="T92" s="28">
+      <c r="T98" s="28">
         <v>10554472</v>
       </c>
     </row>
-    <row r="116" spans="3:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="117" spans="3:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E117" s="1" t="s">
+    <row r="122" spans="3:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="123" spans="3:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E123" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="F117" s="2"/>
-      <c r="G117" s="3"/>
-      <c r="H117" s="1" t="s">
+      <c r="F123" s="2"/>
+      <c r="G123" s="3"/>
+      <c r="H123" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="I117" s="2"/>
-      <c r="J117" s="3"/>
+      <c r="I123" s="2"/>
+      <c r="J123" s="3"/>
     </row>
-    <row r="118" spans="3:10" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D118" s="4"/>
-      <c r="E118" s="5" t="s">
+    <row r="124" spans="3:10" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D124" s="4"/>
+      <c r="E124" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="F118" s="6" t="s">
+      <c r="F124" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="G118" s="7" t="s">
+      <c r="G124" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="H118" s="8" t="s">
+      <c r="H124" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="I118" s="9" t="s">
+      <c r="I124" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="J118" s="10" t="s">
+      <c r="J124" s="10" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="119" spans="3:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C119" s="67" t="s">
+    <row r="125" spans="3:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C125" s="67" t="s">
         <v>2</v>
       </c>
-      <c r="D119" s="23" t="s">
+      <c r="D125" s="23" t="s">
         <v>15</v>
       </c>
-      <c r="E119" s="24">
+      <c r="E125" s="24">
         <v>0.92668473911135196</v>
       </c>
-      <c r="F119" s="25">
+      <c r="F125" s="25">
         <v>1.05909783386849E-2</v>
       </c>
-      <c r="G119" s="26">
+      <c r="G125" s="26">
         <v>968325</v>
       </c>
-      <c r="H119" s="45">
+      <c r="H125" s="45">
         <v>0.92779677610091504</v>
       </c>
-      <c r="I119" s="47">
+      <c r="I125" s="47">
         <v>3.6682658956604798E-3</v>
       </c>
-      <c r="J119" s="46">
+      <c r="J125" s="46">
         <v>6484198</v>
       </c>
     </row>
-    <row r="120" spans="3:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C120" s="67"/>
-      <c r="D120" s="23" t="s">
+    <row r="126" spans="3:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C126" s="67"/>
+      <c r="D126" s="23" t="s">
         <v>16</v>
       </c>
-      <c r="E120" s="24">
+      <c r="E126" s="24">
         <v>0.69307009183924895</v>
       </c>
-      <c r="F120" s="25">
+      <c r="F126" s="25">
         <v>1.73185149047532E-2</v>
       </c>
-      <c r="G120" s="26">
+      <c r="G126" s="26">
         <v>1160506</v>
       </c>
-      <c r="H120" s="51">
+      <c r="H126" s="51">
         <v>0.75566507798009697</v>
       </c>
-      <c r="I120" s="52">
+      <c r="I126" s="52">
         <v>5.4472118452649296E-3</v>
       </c>
-      <c r="J120" s="53">
+      <c r="J126" s="53">
         <v>7977869</v>
       </c>
     </row>
-    <row r="121" spans="3:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C121" s="67" t="s">
+    <row r="127" spans="3:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C127" s="67" t="s">
         <v>3</v>
       </c>
-      <c r="D121" s="31" t="s">
+      <c r="D127" s="31" t="s">
         <v>15</v>
       </c>
-      <c r="E121" s="39">
+      <c r="E127" s="39">
         <v>0.72742104358135695</v>
       </c>
-      <c r="F121" s="41">
+      <c r="F127" s="41">
         <v>1.3783532832492101E-2</v>
       </c>
-      <c r="G121" s="40">
+      <c r="G127" s="40">
         <v>2157551</v>
       </c>
-      <c r="H121" s="49">
+      <c r="H127" s="49">
         <v>0.72201975027028897</v>
       </c>
-      <c r="I121" s="50">
+      <c r="I127" s="50">
         <v>5.3424684010458098E-3</v>
       </c>
-      <c r="J121" s="48">
+      <c r="J127" s="48">
         <v>14163553</v>
       </c>
     </row>
-    <row r="122" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C122" s="67"/>
-      <c r="D122" s="31" t="s">
+    <row r="128" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C128" s="67"/>
+      <c r="D128" s="31" t="s">
         <v>16</v>
       </c>
-      <c r="E122" s="42">
+      <c r="E128" s="42">
         <v>0.69684902421049899</v>
       </c>
-      <c r="F122" s="43">
+      <c r="F128" s="43">
         <v>1.4223407773721899E-2</v>
       </c>
-      <c r="G122" s="44">
+      <c r="G128" s="44">
         <v>1963487</v>
       </c>
-      <c r="H122" s="54">
+      <c r="H128" s="54">
         <v>0.695811478623517</v>
       </c>
-      <c r="I122" s="55">
+      <c r="I128" s="55">
         <v>4.4586455593805798E-3</v>
       </c>
-      <c r="J122" s="56">
+      <c r="J128" s="56">
         <v>12844676</v>
       </c>
     </row>
-    <row r="148" spans="3:12" x14ac:dyDescent="0.25">
-      <c r="C148" t="s">
+    <row r="154" spans="3:12" x14ac:dyDescent="0.25">
+      <c r="C154" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="150" spans="3:12" x14ac:dyDescent="0.25">
-      <c r="E150" t="s">
+    <row r="156" spans="3:12" x14ac:dyDescent="0.25">
+      <c r="E156" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="151" spans="3:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D151" s="66" t="s">
+    <row r="157" spans="3:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D157" s="66" t="s">
         <v>27</v>
       </c>
-      <c r="E151" s="66"/>
-      <c r="F151" s="66" t="s">
+      <c r="E157" s="66"/>
+      <c r="F157" s="66" t="s">
         <v>26</v>
       </c>
-      <c r="G151" s="66"/>
-      <c r="H151" s="64"/>
-      <c r="I151" s="64"/>
+      <c r="G157" s="66"/>
+      <c r="H157" s="64"/>
+      <c r="I157" s="64"/>
     </row>
-    <row r="152" spans="3:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D152" s="1" t="s">
+    <row r="158" spans="3:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D158" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E152" s="58" t="s">
+      <c r="E158" s="58" t="s">
         <v>3</v>
       </c>
-      <c r="F152" s="1" t="s">
+      <c r="F158" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="G152" s="58" t="s">
+      <c r="G158" s="58" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="153" spans="3:12" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C153" s="36"/>
-      <c r="D153" s="7" t="s">
+    <row r="159" spans="3:12" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C159" s="36"/>
+      <c r="D159" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="E153" s="10" t="s">
+      <c r="E159" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="F153" s="57" t="s">
+      <c r="F159" s="57" t="s">
         <v>6</v>
       </c>
-      <c r="G153" s="60" t="s">
+      <c r="G159" s="60" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="154" spans="3:12" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C154" s="37" t="s">
+    <row r="160" spans="3:12" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C160" s="37" t="s">
         <v>28</v>
       </c>
-      <c r="D154" s="34">
+      <c r="D160" s="34">
         <v>1181</v>
       </c>
-      <c r="E154" s="35">
+      <c r="E160" s="35">
         <v>127791</v>
       </c>
-      <c r="F154" s="63">
+      <c r="F160" s="63">
         <v>2406</v>
       </c>
-      <c r="G154" s="62">
+      <c r="G160" s="62">
         <v>713128</v>
       </c>
-      <c r="I154" s="65">
-        <f>D154/SUM(D$154:D$158)</f>
+      <c r="I160" s="65">
+        <f>D160/SUM(D$160:D$164)</f>
         <v>1.0176595381669719E-3</v>
       </c>
-      <c r="J154" s="65">
-        <f t="shared" ref="J154:L158" si="17">E154/SUM(E$154:E$158)</f>
+      <c r="J160" s="65">
+        <f t="shared" ref="J160:L164" si="17">E160/SUM(E$160:E$164)</f>
         <v>6.5083700579632059E-2</v>
       </c>
-      <c r="K154" s="65">
+      <c r="K160" s="65">
         <f t="shared" si="17"/>
         <v>3.0158429525478544E-4</v>
       </c>
-      <c r="L154" s="65">
+      <c r="L160" s="65">
         <f t="shared" si="17"/>
         <v>5.5519345135681117E-2</v>
       </c>
     </row>
-    <row r="155" spans="3:12" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C155" s="37" t="s">
+    <row r="161" spans="3:12" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C161" s="37" t="s">
         <v>29</v>
       </c>
-      <c r="D155" s="26">
+      <c r="D161" s="26">
         <v>19494</v>
       </c>
-      <c r="E155" s="28">
+      <c r="E161" s="28">
         <v>383792</v>
       </c>
-      <c r="F155" s="61">
+      <c r="F161" s="61">
         <v>221947</v>
       </c>
-      <c r="G155" s="59">
+      <c r="G161" s="59">
         <v>2399574</v>
       </c>
-      <c r="I155" s="65">
-        <f t="shared" ref="I155:I158" si="18">D155/SUM(D$154:D$158)</f>
+      <c r="I161" s="65">
+        <f t="shared" ref="I161:I164" si="18">D161/SUM(D$160:D$164)</f>
         <v>1.6797845077922906E-2</v>
       </c>
-      <c r="J155" s="65">
+      <c r="J161" s="65">
         <f t="shared" si="17"/>
         <v>0.19546449760044249</v>
       </c>
-      <c r="K155" s="65">
+      <c r="K161" s="65">
         <f t="shared" si="17"/>
         <v>2.7820336483339096E-2</v>
       </c>
-      <c r="L155" s="65">
+      <c r="L161" s="65">
         <f t="shared" si="17"/>
         <v>0.18681467714716976</v>
       </c>
     </row>
-    <row r="156" spans="3:12" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C156" s="37" t="s">
+    <row r="162" spans="3:12" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C162" s="37" t="s">
         <v>30</v>
       </c>
-      <c r="D156" s="26">
+      <c r="D162" s="26">
         <v>208032</v>
       </c>
-      <c r="E156" s="28">
+      <c r="E162" s="28">
         <v>576634</v>
       </c>
-      <c r="F156" s="61">
+      <c r="F162" s="61">
         <v>1998546</v>
       </c>
-      <c r="G156" s="59">
+      <c r="G162" s="59">
         <v>2418598</v>
       </c>
-      <c r="I156" s="65">
+      <c r="I162" s="65">
         <f t="shared" si="18"/>
         <v>0.17925973670105971</v>
       </c>
-      <c r="J156" s="65">
+      <c r="J162" s="65">
         <f t="shared" si="17"/>
         <v>0.2936785423076394</v>
       </c>
-      <c r="K156" s="65">
+      <c r="K162" s="65">
         <f t="shared" si="17"/>
         <v>0.25051125808157543</v>
       </c>
-      <c r="L156" s="65">
+      <c r="L162" s="65">
         <f t="shared" si="17"/>
         <v>0.18829575771315679</v>
       </c>
     </row>
-    <row r="157" spans="3:12" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C157" s="37" t="s">
+    <row r="163" spans="3:12" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C163" s="37" t="s">
         <v>31</v>
       </c>
-      <c r="D157" s="26">
+      <c r="D163" s="26">
         <v>758924</v>
       </c>
-      <c r="E157" s="28">
+      <c r="E163" s="28">
         <v>296755</v>
       </c>
-      <c r="F157" s="61">
+      <c r="F163" s="61">
         <v>4665672</v>
       </c>
-      <c r="G157" s="59">
+      <c r="G163" s="59">
         <v>1745044</v>
       </c>
-      <c r="I157" s="65">
+      <c r="I163" s="65">
         <f t="shared" si="18"/>
         <v>0.65395956591348947</v>
       </c>
-      <c r="J157" s="65">
+      <c r="J163" s="65">
         <f t="shared" si="17"/>
         <v>0.15113672766868333</v>
       </c>
-      <c r="K157" s="65">
+      <c r="K163" s="65">
         <f t="shared" si="17"/>
         <v>0.58482685037821502</v>
       </c>
-      <c r="L157" s="65">
+      <c r="L163" s="65">
         <f t="shared" si="17"/>
         <v>0.13585737779606119</v>
       </c>
     </row>
-    <row r="158" spans="3:12" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C158" s="37" t="s">
+    <row r="164" spans="3:12" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C164" s="37" t="s">
         <v>32</v>
       </c>
-      <c r="D158" s="26">
+      <c r="D164" s="26">
         <v>172875</v>
       </c>
-      <c r="E158" s="28">
+      <c r="E164" s="28">
         <v>578515</v>
       </c>
-      <c r="F158" s="61">
+      <c r="F164" s="61">
         <v>1089298</v>
       </c>
-      <c r="G158" s="59">
+      <c r="G164" s="59">
         <v>5568332</v>
       </c>
-      <c r="I158" s="65">
+      <c r="I164" s="65">
         <f t="shared" si="18"/>
         <v>0.14896519276936096</v>
       </c>
-      <c r="J158" s="65">
+      <c r="J164" s="65">
         <f t="shared" si="17"/>
         <v>0.29463653184360272</v>
       </c>
-      <c r="K158" s="65">
+      <c r="K164" s="65">
         <f t="shared" si="17"/>
         <v>0.13653997076161567</v>
       </c>
-      <c r="L158" s="65">
+      <c r="L164" s="65">
         <f t="shared" si="17"/>
         <v>0.43351284220793113</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="4">
-    <mergeCell ref="D151:E151"/>
-    <mergeCell ref="F151:G151"/>
-    <mergeCell ref="C121:C122"/>
-    <mergeCell ref="C119:C120"/>
+    <mergeCell ref="D157:E157"/>
+    <mergeCell ref="F157:G157"/>
+    <mergeCell ref="C127:C128"/>
+    <mergeCell ref="C125:C126"/>
   </mergeCells>
-  <conditionalFormatting sqref="B57:G57 B89:H92">
+  <conditionalFormatting sqref="B63:G63 B95:H98">
     <cfRule type="expression" dxfId="10" priority="17">
-      <formula>ISERROR($F57)</formula>
+      <formula>ISERROR($F63)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B58:G58">
+  <conditionalFormatting sqref="B64:G64">
     <cfRule type="expression" dxfId="9" priority="16">
-      <formula>ISERROR($F58)</formula>
+      <formula>ISERROR($F64)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B59:G59">
+  <conditionalFormatting sqref="B65:G65">
     <cfRule type="expression" dxfId="8" priority="15">
-      <formula>ISERROR($F59)</formula>
+      <formula>ISERROR($F65)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="O89:S89">
+  <conditionalFormatting sqref="O95:S95">
     <cfRule type="expression" dxfId="7" priority="12">
-      <formula>ISERROR($F89)</formula>
+      <formula>ISERROR($F95)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="O90:S90">
+  <conditionalFormatting sqref="O96:S96">
     <cfRule type="expression" dxfId="6" priority="11">
-      <formula>ISERROR($F90)</formula>
+      <formula>ISERROR($F96)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="O91:S91">
+  <conditionalFormatting sqref="O97:S97">
     <cfRule type="expression" dxfId="5" priority="10">
-      <formula>ISERROR($F91)</formula>
+      <formula>ISERROR($F97)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="O92:S92">
+  <conditionalFormatting sqref="O98:S98">
     <cfRule type="expression" dxfId="4" priority="9">
-      <formula>ISERROR($F92)</formula>
+      <formula>ISERROR($F98)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E121:I122">
+  <conditionalFormatting sqref="E127:I128">
     <cfRule type="expression" dxfId="3" priority="18">
-      <formula>ISERROR($H121)</formula>
+      <formula>ISERROR($H127)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D121:D122">
+  <conditionalFormatting sqref="D127:D128">
     <cfRule type="expression" dxfId="2" priority="5">
-      <formula>ISERROR($H121)</formula>
+      <formula>ISERROR($H127)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C154:D158">
+  <conditionalFormatting sqref="C160:D164">
     <cfRule type="expression" dxfId="1" priority="20">
       <formula>ISERROR(#REF!)</formula>
     </cfRule>

</xml_diff>

<commit_message>
crappy commit as restore i not working
</commit_message>
<xml_diff>
--- a/OUTPUT/DATA/Charting.xlsx
+++ b/OUTPUT/DATA/Charting.xlsx
@@ -12122,4 +12122,264 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100535EDF9DD8DBB143AE8CD71BDB6B0E3B" ma:contentTypeVersion="16" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="58db4c0cb4a6c8574584e2b7e3b481f7">
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="7fc9ebc1-6786-4aad-aee1-fdcde6e01ff9" xmlns:ns3="fd7425d0-09b7-49b7-b351-1ad2162dc0d7" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="7f205f5aa0458c3a5f4d8c0367cd4bd4" ns2:_="" ns3:_="">
+    <xsd:import namespace="7fc9ebc1-6786-4aad-aee1-fdcde6e01ff9"/>
+    <xsd:import namespace="fd7425d0-09b7-49b7-b351-1ad2162dc0d7"/>
+    <xsd:element name="properties">
+      <xsd:complexType>
+        <xsd:sequence>
+          <xsd:element name="documentManagement">
+            <xsd:complexType>
+              <xsd:all>
+                <xsd:element ref="ns2:MediaServiceMetadata" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceFastMetadata" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceAutoKeyPoints" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceKeyPoints" minOccurs="0"/>
+                <xsd:element ref="ns3:SharedWithUsers" minOccurs="0"/>
+                <xsd:element ref="ns3:SharedWithDetails" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceAutoTags" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceOCR" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceGenerationTime" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceEventHashCode" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceDateTaken" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaLengthInSeconds" minOccurs="0"/>
+                <xsd:element ref="ns2:lcf76f155ced4ddcb4097134ff3c332f" minOccurs="0"/>
+                <xsd:element ref="ns3:TaxCatchAll" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceLocation" minOccurs="0"/>
+              </xsd:all>
+            </xsd:complexType>
+          </xsd:element>
+        </xsd:sequence>
+      </xsd:complexType>
+    </xsd:element>
+  </xsd:schema>
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="7fc9ebc1-6786-4aad-aee1-fdcde6e01ff9" elementFormDefault="qualified">
+    <xsd:import namespace="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <xsd:import namespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <xsd:element name="MediaServiceMetadata" ma:index="8" nillable="true" ma:displayName="MediaServiceMetadata" ma:hidden="true" ma:internalName="MediaServiceMetadata" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceFastMetadata" ma:index="9" nillable="true" ma:displayName="MediaServiceFastMetadata" ma:hidden="true" ma:internalName="MediaServiceFastMetadata" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceAutoKeyPoints" ma:index="10" nillable="true" ma:displayName="MediaServiceAutoKeyPoints" ma:hidden="true" ma:internalName="MediaServiceAutoKeyPoints" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceKeyPoints" ma:index="11" nillable="true" ma:displayName="KeyPoints" ma:internalName="MediaServiceKeyPoints" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note">
+          <xsd:maxLength value="255"/>
+        </xsd:restriction>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceAutoTags" ma:index="14" nillable="true" ma:displayName="Tags" ma:internalName="MediaServiceAutoTags" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceOCR" ma:index="15" nillable="true" ma:displayName="Extracted Text" ma:internalName="MediaServiceOCR" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note">
+          <xsd:maxLength value="255"/>
+        </xsd:restriction>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceGenerationTime" ma:index="16" nillable="true" ma:displayName="MediaServiceGenerationTime" ma:hidden="true" ma:internalName="MediaServiceGenerationTime" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceEventHashCode" ma:index="17" nillable="true" ma:displayName="MediaServiceEventHashCode" ma:hidden="true" ma:internalName="MediaServiceEventHashCode" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceDateTaken" ma:index="18" nillable="true" ma:displayName="MediaServiceDateTaken" ma:hidden="true" ma:internalName="MediaServiceDateTaken" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaLengthInSeconds" ma:index="19" nillable="true" ma:displayName="Length (seconds)" ma:internalName="MediaLengthInSeconds" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Unknown"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="lcf76f155ced4ddcb4097134ff3c332f" ma:index="21" nillable="true" ma:taxonomy="true" ma:internalName="lcf76f155ced4ddcb4097134ff3c332f" ma:taxonomyFieldName="MediaServiceImageTags" ma:displayName="Image Tags" ma:readOnly="false" ma:fieldId="{5cf76f15-5ced-4ddc-b409-7134ff3c332f}" ma:taxonomyMulti="true" ma:sspId="5651981c-07c9-48be-a366-aa18a08a6388" ma:termSetId="09814cd3-568e-fe90-9814-8d621ff8fb84" ma:anchorId="fba54fb3-c3e1-fe81-a776-ca4b69148c4d" ma:open="true" ma:isKeyword="false">
+      <xsd:complexType>
+        <xsd:sequence>
+          <xsd:element ref="pc:Terms" minOccurs="0" maxOccurs="1"/>
+        </xsd:sequence>
+      </xsd:complexType>
+    </xsd:element>
+    <xsd:element name="MediaServiceLocation" ma:index="23" nillable="true" ma:displayName="Location" ma:description="" ma:indexed="true" ma:internalName="MediaServiceLocation" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+  </xsd:schema>
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="fd7425d0-09b7-49b7-b351-1ad2162dc0d7" elementFormDefault="qualified">
+    <xsd:import namespace="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <xsd:import namespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <xsd:element name="SharedWithUsers" ma:index="12" nillable="true" ma:displayName="Shared With" ma:internalName="SharedWithUsers" ma:readOnly="true">
+      <xsd:complexType>
+        <xsd:complexContent>
+          <xsd:extension base="dms:UserMulti">
+            <xsd:sequence>
+              <xsd:element name="UserInfo" minOccurs="0" maxOccurs="unbounded">
+                <xsd:complexType>
+                  <xsd:sequence>
+                    <xsd:element name="DisplayName" type="xsd:string" minOccurs="0"/>
+                    <xsd:element name="AccountId" type="dms:UserId" minOccurs="0" nillable="true"/>
+                    <xsd:element name="AccountType" type="xsd:string" minOccurs="0"/>
+                  </xsd:sequence>
+                </xsd:complexType>
+              </xsd:element>
+            </xsd:sequence>
+          </xsd:extension>
+        </xsd:complexContent>
+      </xsd:complexType>
+    </xsd:element>
+    <xsd:element name="SharedWithDetails" ma:index="13" nillable="true" ma:displayName="Shared With Details" ma:internalName="SharedWithDetails" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note">
+          <xsd:maxLength value="255"/>
+        </xsd:restriction>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="TaxCatchAll" ma:index="22" nillable="true" ma:displayName="Taxonomy Catch All Column" ma:hidden="true" ma:list="{20544d0c-2e96-4949-8e6e-e90d9b14e1b3}" ma:internalName="TaxCatchAll" ma:showField="CatchAllData" ma:web="fd7425d0-09b7-49b7-b351-1ad2162dc0d7">
+      <xsd:complexType>
+        <xsd:complexContent>
+          <xsd:extension base="dms:MultiChoiceLookup">
+            <xsd:sequence>
+              <xsd:element name="Value" type="dms:Lookup" maxOccurs="unbounded" minOccurs="0" nillable="true"/>
+            </xsd:sequence>
+          </xsd:extension>
+        </xsd:complexContent>
+      </xsd:complexType>
+    </xsd:element>
+  </xsd:schema>
+  <xsd:schema xmlns="http://schemas.openxmlformats.org/package/2006/metadata/core-properties" xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:dc="http://purl.org/dc/elements/1.1/" xmlns:dcterms="http://purl.org/dc/terms/" xmlns:odoc="http://schemas.microsoft.com/internal/obd" targetNamespace="http://schemas.openxmlformats.org/package/2006/metadata/core-properties" elementFormDefault="qualified" attributeFormDefault="unqualified" blockDefault="#all">
+    <xsd:import namespace="http://purl.org/dc/elements/1.1/" schemaLocation="http://dublincore.org/schemas/xmls/qdc/2003/04/02/dc.xsd"/>
+    <xsd:import namespace="http://purl.org/dc/terms/" schemaLocation="http://dublincore.org/schemas/xmls/qdc/2003/04/02/dcterms.xsd"/>
+    <xsd:element name="coreProperties" type="CT_coreProperties"/>
+    <xsd:complexType name="CT_coreProperties">
+      <xsd:all>
+        <xsd:element ref="dc:creator" minOccurs="0" maxOccurs="1"/>
+        <xsd:element ref="dcterms:created" minOccurs="0" maxOccurs="1"/>
+        <xsd:element ref="dc:identifier" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="contentType" minOccurs="0" maxOccurs="1" type="xsd:string" ma:index="0" ma:displayName="Content Type"/>
+        <xsd:element ref="dc:title" minOccurs="0" maxOccurs="1" ma:index="4" ma:displayName="Title"/>
+        <xsd:element ref="dc:subject" minOccurs="0" maxOccurs="1"/>
+        <xsd:element ref="dc:description" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="keywords" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element ref="dc:language" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="category" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element name="version" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element name="revision" minOccurs="0" maxOccurs="1" type="xsd:string">
+          <xsd:annotation>
+            <xsd:documentation>
+                        This value indicates the number of saves or revisions. The application is responsible for updating this value after each revision.
+                    </xsd:documentation>
+          </xsd:annotation>
+        </xsd:element>
+        <xsd:element name="lastModifiedBy" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element ref="dcterms:modified" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="contentStatus" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+      </xsd:all>
+    </xsd:complexType>
+  </xsd:schema>
+  <xs:schema xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" xmlns:xs="http://www.w3.org/2001/XMLSchema" targetNamespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" elementFormDefault="qualified" attributeFormDefault="unqualified">
+    <xs:element name="Person">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:DisplayName" minOccurs="0"/>
+          <xs:element ref="pc:AccountId" minOccurs="0"/>
+          <xs:element ref="pc:AccountType" minOccurs="0"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="DisplayName" type="xs:string"/>
+    <xs:element name="AccountId" type="xs:string"/>
+    <xs:element name="AccountType" type="xs:string"/>
+    <xs:element name="BDCAssociatedEntity">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:BDCEntity" minOccurs="0" maxOccurs="unbounded"/>
+        </xs:sequence>
+        <xs:attribute ref="pc:EntityNamespace"/>
+        <xs:attribute ref="pc:EntityName"/>
+        <xs:attribute ref="pc:SystemInstanceName"/>
+        <xs:attribute ref="pc:AssociationName"/>
+      </xs:complexType>
+    </xs:element>
+    <xs:attribute name="EntityNamespace" type="xs:string"/>
+    <xs:attribute name="EntityName" type="xs:string"/>
+    <xs:attribute name="SystemInstanceName" type="xs:string"/>
+    <xs:attribute name="AssociationName" type="xs:string"/>
+    <xs:element name="BDCEntity">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:EntityDisplayName" minOccurs="0"/>
+          <xs:element ref="pc:EntityInstanceReference" minOccurs="0"/>
+          <xs:element ref="pc:EntityId1" minOccurs="0"/>
+          <xs:element ref="pc:EntityId2" minOccurs="0"/>
+          <xs:element ref="pc:EntityId3" minOccurs="0"/>
+          <xs:element ref="pc:EntityId4" minOccurs="0"/>
+          <xs:element ref="pc:EntityId5" minOccurs="0"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="EntityDisplayName" type="xs:string"/>
+    <xs:element name="EntityInstanceReference" type="xs:string"/>
+    <xs:element name="EntityId1" type="xs:string"/>
+    <xs:element name="EntityId2" type="xs:string"/>
+    <xs:element name="EntityId3" type="xs:string"/>
+    <xs:element name="EntityId4" type="xs:string"/>
+    <xs:element name="EntityId5" type="xs:string"/>
+    <xs:element name="Terms">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:TermInfo" minOccurs="0" maxOccurs="unbounded"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="TermInfo">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:TermName" minOccurs="0"/>
+          <xs:element ref="pc:TermId" minOccurs="0"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="TermName" type="xs:string"/>
+    <xs:element name="TermId" type="xs:string"/>
+  </xs:schema>
+</ct:contentTypeSchema>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{555B8F3F-4A26-4C57-B800-D010422B89BB}"/>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1BA92396-96B6-4A6B-9118-3D6469E5AB05}"/>
 </file>
</xml_diff>